<commit_message>
Updated Excel file with better hand curated question answer pairs
</commit_message>
<xml_diff>
--- a/kedronlp/notebooks/Evaluation.xlsx
+++ b/kedronlp/notebooks/Evaluation.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arjan/Bachelor/NLP with Transformers/pubMedNLP/kedronlp/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBC21D1-8F89-824E-BFE3-3C13251D0B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255BEEDB-53A9-F447-B260-630D2CD314EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16120" activeTab="1" xr2:uid="{3AC1803B-D431-F74E-BDCB-3D80AD30DE94}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16120" xr2:uid="{3AC1803B-D431-F74E-BDCB-3D80AD30DE94}"/>
   </bookViews>
   <sheets>
     <sheet name="Human" sheetId="3" r:id="rId1"/>
     <sheet name="Model" sheetId="1" r:id="rId2"/>
+    <sheet name="Additional" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="376">
   <si>
     <t>Question Type</t>
   </si>
@@ -87,9 +88,6 @@
 Keywords: Brain connectivity; Cognitive reserve; Functional connectivity; Graph theory; Intelligence; Resting state; Robustness; fMRI.</t>
   </si>
   <si>
-    <t>How does the study quantitatively demonstrate the relationship between IQ and brain resilience?</t>
-  </si>
-  <si>
     <t>Yes/No question</t>
   </si>
   <si>
@@ -126,9 +124,6 @@
     <t>What</t>
   </si>
   <si>
-    <t>What evidence does the study provide to support the use of new tools for measuring mindsets in medical education?</t>
-  </si>
-  <si>
     <t>Which</t>
   </si>
   <si>
@@ -148,9 +143,6 @@
   </si>
   <si>
     <t>How</t>
-  </si>
-  <si>
-    <t>How did the researchers measure the clinical supervisors' mindsets?</t>
   </si>
   <si>
     <t xml:space="preserve">For humans, there appears to be a clear link between general intelligence and self-control behavior, such as sustained delay of gratification [1-9]. Chimpanzees also delay gratification [10-12] and can be given tests of general intelligence (g) [13-15], but these two constructs have never been compared within the same sample of nonhuman animals. We presented 40 chimpanzees with the hybrid delay task (HDT) [16, 17], which measures inter-temporal choices and the capacity for sustained delay of gratification, and the primate cognitive test battery (PCTB), which measures g in chimpanzees [13-15]. Importantly, none of the sub-tasks in the PCTB directly assesses self-control or other forms of behavioral inhibition. Rather, they assess areas of physical cognition (e.g., quantity discrimination) or social cognition (e.g., gaze following). In three phases of testing, we consistently found that the strongest relation was between chimpanzee g scores and efficiency in the HDT. Chimpanzee g was not most closely related to the proportion of trials the chimpanzees chose to try to wait for delayed rewards, but rather most closely related to how good they were at waiting for those rewards when they chose to do so. We also found the same strong relation between HDT efficiency and those factors in the PCTB that loaded most strongly on chimpanzee g. These results highlight that, as with humans, there is a strong relation between chimpanzees' self-control and overall intelligence-a relation that likely reflects the role of successful inhibitory control during cognitive processing of information and intelligent decision-making.
@@ -220,13 +212,6 @@
     <t>Can an individual's "Mind-space" model change or evolve over time?</t>
   </si>
   <si>
-    <t>According to the study, which of the following is the primary factor influencing the accuracy of mental state inferences?
-a) The number of dimensions used in an individual's "Mind-space" model
-b) The accuracy of an individual's model of how minds covary
-c) The ability to locate a specific mind within one's "Mind-space"
-d) Pre-existing biases about other people's mental states</t>
-  </si>
-  <si>
     <t>Intelligent life has emerged late in Earth's habitable lifetime, and required a preceding series of key evolutionary transitions. A simple model (the Carter model) explains the late arrival of intelligent life by positing these evolutionary transitions were exceptionally unlikely 'critical steps'. An alternative model (the neocatastrophism hypothesis) proposes that intelligent life was delayed by frequent catastrophes that served to set back evolutionary innovation. Here, we generalize the Carter model and explore this hypothesis by including catastrophes that can 'undo' an evolutionary transition. Introducing catastrophes or evolutionary dead ends can create situations in which critical steps occur rapidly or in clusters, suggesting that past estimates of the number of critical steps could be underestimated. If catastrophes affect complex life more than simple life, the critical steps will also exhibit a pattern of acceleration towards the present, suggesting that the increase in biological complexity over the past 500 Myr could reflect previously overlooked evolutionary transitions. Furthermore, our results have implications for understanding the different explanations (critical steps versus neo-catastrophes) for the evolution of intelligent life and the so-called Fermi paradox-the observation that intelligent life appears rare in the observable Universe.</t>
   </si>
   <si>
@@ -248,13 +233,6 @@
     <t>Do the factors predicting heroin DD in a state of satiation differ completely from those predicting DD in a state of withdrawal?</t>
   </si>
   <si>
-    <t>Which of the following best summarizes the primary finding of the study?
-a) Heroin delay discounting is not influenced by pharmacological state.
-b) Delay discounting is a trait that remains constant regardless of circumstances.
-c) Heroin delay discounting is influenced by both pharmacological state and individual characteristics.
-d) Intelligence is the single greatest predictor of heroin delay discounting.</t>
-  </si>
-  <si>
     <t>The continuous development of the society has led to the improvement of people's quality of life and consumption level. At the same time, peoples demand for all aspects of production and life is also increasing, thus promoting the emergence and innovation of intelligent household appliances. To manage these devices conveniently and quickly and enrich family life, "smart home" bureau plays a very important role. Smart home, which enters people's family life, uses communication technology, Internet connection technology, automatic fire control technology, network wiring technology, and visual and audio transmission technology to communicate with home. Mobile terminals have been developed, and more and more PC functions have been realized. Based on the hardware platform of the smart home management system, two solutions were put forward. The first solution is combined with the current 5G network, and through it, the user can control the mobile phone and other mobile terminals on the corresponding application operation instructions to create. The second solution is the design of the web server intelligent management system, for relevant information. It is collected into the database of the server, allows remote access to the node and subscriber information related to storage in the database through the Internet, and searches the information to control the home lighting and temperature. This system is designed to imitate the modular scheme, which includes the central control module, sensor data acquisition module, and software module. Finally, on the browser side and the electronic devices of Android operating system, it realizes the wireless control of lighting, air conditioning, washing machine, and other devices, as well as the detection of the home environment.</t>
   </si>
   <si>
@@ -267,18 +245,9 @@
     <t>When might a user choose to control their smart home devices from a mobile terminal versus a web interface?</t>
   </si>
   <si>
-    <t>Who are the intended users of this smart home system?</t>
-  </si>
-  <si>
-    <t>How does the system enable control of lighting, air conditioning, and other appliances?</t>
-  </si>
-  <si>
     <t>Target-driven visual navigation is essential for many applications in robotics, and it has gained increasing interest in recent years. In this work, inspired by animal cognitive mechanisms, we propose a novel navigation architecture that simultaneously learns exploration policy and encodes environmental structure. First, to learn exploration policy directly from raw visual input, we use deep reinforcement learning as the basic framework and allow agents to create rewards for themselves as learning signals. In our approach, the reward for the current observation is driven by curiosity and calculated by a count-based approach and temporal distance. While agents learn exploration policy, we use temporal distance to find waypoints in observation sequences and incrementally describe the structure of the environment in a way that integrates episodic memory. Finally, space topological cognition is integrated into the model as a path planning module and combined with a locomotion network to obtain a more generalized approach to navigation. We test our approach in the DMlab, a visually rich 3D environment, and validate its exploration efficiency and navigation performance through extensive experiments. The experimental results show that our approach can explore and encode the environment more efficiently and has better capability in dealing with stochastic objects. In navigation tasks, agents can use space topological cognition to effectively reach the target and guide detour behaviour when a path is unavailable, exhibiting good environmental adaptability.</t>
   </si>
   <si>
-    <t>What is the purpose of integrating space topological cognition into the model?</t>
-  </si>
-  <si>
     <t>Which component of the architecture is responsible for guiding detour behavior?</t>
   </si>
   <si>
@@ -298,12 +267,6 @@
   </si>
   <si>
     <t>Many studies have reported attentional biases based on feature-reward associations. However, the effects of location-reward associations on attentional selection remain less well-understood. Unlike feature cases, a previous study that induced participants' awareness of the location-reward association by instructing them to look for a high-reward location has suggested the critical role of goal-driven manipulations in such associations. In this study, we investigated whether the reward effect occurred without goal-driven manipulations if participants were spontaneously aware of the location-reward association. We conducted three experiments using a visual search task that included four circles where participants received rewards; one possible target location was associated with a high reward, and another with a low reward. In Experiment 1, the target was presented among distractors, and participants had to search for the target. The results showed a faster reaction time in the high-reward rather than the low-reward locations only in participants aware of the location-reward association, even if they were not required to look for the association. Moreover, in Experiment 2, we replicated the main findings of Experiment 1, even when the target had an abrupt visual onset to restrict goal-driven manipulations. Furthermore, Experiment 3 confirmed that the effect observed in Experiment 2 could not be attributed to the initial eye position. These findings suggest that goal-driven manipulations are unnecessary for inducing reward biases to high-reward locations. We concluded that awareness of the association rather than goal-driven manipulations is crucial for the location-reward effect.</t>
-  </si>
-  <si>
-    <t>How does the study challenge previous findings about the role of goal-driven manipulation in location-reward association?</t>
-  </si>
-  <si>
-    <t>Did the researchers find a significant location-reward effect even when participants were not actively searching for high-reward locations?</t>
   </si>
   <si>
     <t>Which factor appears to be the most important for inducing a reward bias in the study?
@@ -325,9 +288,6 @@
     <t>Who were the primary beneficiaries of the health mediator's work?</t>
   </si>
   <si>
-    <t>How did the health mediators' work increase their self-esteem and social status?</t>
-  </si>
-  <si>
     <t>Why is the use of health mediators particularly important in areas with disadvantaged Roma populations?</t>
   </si>
   <si>
@@ -358,16 +318,10 @@
     <t>Although providing negative performance feedback can enhance employee performance, leaders are sometimes reluctant to engage in this activity. Reflecting this, prior research has identified negative feedback provision as an aversive, yet potentially rewarding, managerial activity. However, little is known about how providing negative feedback impacts the effectiveness of leaders who do so. To shed light on this issue, we develop and test a theoretical model that identifies how leaders' proximal and distal reactions to providing negative feedback are contingent upon their levels of trait empathy. Supporting our theory, results from an experience sampling study indicate that leaders higher in trait empathy report feeling both less attentive and more distressed after providing subordinates with negative feedback, whereas leaders lower in trait empathy report feeling more attentive and less distressed. Attentiveness and distress, in turn, were associated with leaders' daily perceptions of their effectiveness; distress was also associated with leaders' daily enactment of transformational leadership behavior. Results of two subsequent studies focused on single episodes of negative feedback provision revealed that trait empathy amplifies the extent to which feedback recipients' negative emotional reactions impact additional leader effectiveness criteria (e.g., executive functioning and planning/problem-solving), further supporting the need to account for the crucial role of trait empathy in the feedback-provision process. Altogether, our research provides a novel perspective on the feedback-giving process by shifting the focus of theorizing from the recipient to the provider, while challenging current thinking about leader empathy by highlighting its potential downside for leadership. (PsycInfo Database Record (c) 2022 APA, all rights reserved).</t>
   </si>
   <si>
-    <t>Does the study suggest that there are potential downsides to leader empathy in the context of giving negative feedback?</t>
-  </si>
-  <si>
     <t>How can nurse leaders use emotional intelligence to specifically address the challenges of stress, exhaustion, and the risk of moral injury brought on by the COVID-19 pandemic?</t>
   </si>
   <si>
     <t>Emotionally intelligent leaders demonstrate a sensitivity to their own and other people's psychological health and well-being, directing others towards common goals while developing effective personal relationships with their colleagues and team members. Emotional intelligence is particularly relevant in the context of the coronavirus disease 2019 pandemic, where nurse leaders need to demonstrate this skill when supporting their teams to manage high levels of stress, exhaustion and the risk of moral injury. This article explores emotional intelligence, discusses its importance as a characteristic of effective nurse leaders and managers, and suggests practical activities that leaders can undertake to develop their emotional intelligence skills.</t>
-  </si>
-  <si>
-    <t>There might be no significant differences in conscientious intelligence sub-dimensions between first and fourth-year nursing students because the study found that factors such as willingness to choose nursing as a profession, gender (female), and not perceiving nursing as solely a means to earn money were more influential in determining conscientious intelligence scores than academic year level.</t>
   </si>
   <si>
     <t>Yes, according to the study, nursing students who do not perceive nursing as solely a means to earn money demonstrate higher levels of conscientious intelligence.</t>
@@ -467,9 +421,6 @@
     <t>No, the factors predicting heroin delay discounting (DD) in a state of satiation partially overlap with those predicting DD in a state of withdrawal. Lower intelligence and higher IRQ Speed (to return to drug use) predicted greater discounting in both states, while lower IRQ Capacity for Delay predicted greater discounting only in the satiation condition.</t>
   </si>
   <si>
-    <t>c) Heroin delay discounting is influenced by both pharmacological state and individual characteristics.</t>
-  </si>
-  <si>
     <t>The smart home system utilizes communication technology, Internet connection technology, automatic fire control technology, network wiring technology, and visual and audio transmission technology.</t>
   </si>
   <si>
@@ -485,9 +436,6 @@
     <t>The system enables control of lighting, air conditioning, and other appliances wirelessly through mobile terminals or web interfaces connected to the smart home management system.</t>
   </si>
   <si>
-    <t>The purpose of integrating space topological cognition into the model is to serve as a path planning module, enabling the model to obtain a more generalized approach to navigation.</t>
-  </si>
-  <si>
     <t>The space topological cognition component is responsible for guiding detour behavior in the navigation architecture.</t>
   </si>
   <si>
@@ -573,9 +521,6 @@
   </si>
   <si>
     <t>What IQ is higher - 100 or 120?</t>
-  </si>
-  <si>
-    <t>Procedural questions</t>
   </si>
   <si>
     <t>An accurate and robust Automatic License Plate Recognition (ALPR) method proves surprising versatility in an Intelligent Transportation and Surveillance (ITS) system. However, most of the existing approaches often use prior knowledge or fixed pre-and-post processing rules and are thus limited by poor generalization in complex real-life conditions. In this paper, we leverage a YOLO-based end-to-end generic ALPR pipeline for vehicle detection (VD), license plate (LP) detection and recognition without exploiting prior knowledge or additional steps in inference. We assess the whole ALPR pipeline, starting from vehicle detection to the LP recognition stage, including a vehicle classifier for emergency vehicles and heavy trucks. We used YOLO v2 in the initial stage of the pipeline and remaining stages are based on the state-of-the-art YOLO v4 detector with various data augmentation and generation techniques to obtain LP recognition accuracy on par with current proposed methods. To evaluate our approach, we used five public datasets from different regions, and we achieved an average recognition accuracy of 90.3% while maintaining an acceptable frames per second (FPS) on a low-end GPU.
@@ -1189,6 +1134,159 @@
   </si>
   <si>
     <t>Answer Human</t>
+  </si>
+  <si>
+    <t>How can we quantitatively demonstrate the relationship between IQ and brain resilience?</t>
+  </si>
+  <si>
+    <t>What evidence is there to support the use of new tools for measuring mindsets in medical education?</t>
+  </si>
+  <si>
+    <t>How do researchers measure the clinical supervisors' mindsets?</t>
+  </si>
+  <si>
+    <t>Which of the following is the primary factor influencing the accuracy of mental state inferences?
+a) The number of dimensions used in an individual's "Mind-space" model
+b) The accuracy of an individual's model of how minds covary
+c) The ability to locate a specific mind within one's "Mind-space"
+d) Pre-existing biases about other people's mental states</t>
+  </si>
+  <si>
+    <t>Which of the following factors was found to be associated with a LATER age of ASD diagnosis?
+A. Higher IQ score
+B. Presence of psychiatric symptoms
+C. Recent birth year
+D. Higher levels of adaptive function</t>
+  </si>
+  <si>
+    <t>Objective: This study sought to identify factors that may be associated with delays in autism spectrum disorder (ASD) diagnosis, including birth cohort, sociodemographic characteristics, and clinical features.
+Methods: Participants included 1716 children and adolescents with ASD enrolled in the Autism Speaks Autism Treatment Network (AS-ATN) between the years 2008 and 2011. Data were collected at enrollment using AS-ATN parent- and clinician-report forms and standardized measures of I.Q., ASD symptoms, adaptive function, and psychiatric symptoms.
+Results: Age at first ASD diagnosis was positively correlated with current age, suggesting a birth cohort effect. Sociodemographic and clinical features were also associated with age at diagnosis, even after controlling for current age. Hierarchical linear regression results showed that older current age, lower socioeconomic status (SES), higher I.Q. score, and lower levels of autism symptoms were associated with later age at initial diagnosis. There was also a significant interaction between current age and I.Q., with higher functioning children being diagnosed at younger ages than in previous years.
+Conclusions: Early diagnosis of ASD is critically important for improving access to interventions; however, many children experience diagnostic delays. In this sample, children from the most recent birth cohorts were diagnosed earlier, suggesting that early signs of ASD are being increasingly recognized. However, socioeconomic barriers to diagnosis still seem to exist. Children with less severe ASD symptoms and with higher I.Q. are also diagnosed at later ages. Efforts are still needed to reduce diagnostic disparities for families of low SES and to improve early recognition of more subtle symptoms.</t>
+  </si>
+  <si>
+    <t>The factor found to be associated with a LATER age of ASD diagnosis in the study was:
+A. Higher IQ score</t>
+  </si>
+  <si>
+    <t>Who are the intended users of a smart home system?</t>
+  </si>
+  <si>
+    <t>How does a smart home system enable control of lighting, air conditioning, and other appliances?</t>
+  </si>
+  <si>
+    <t>How are the previous findings about the role of goal-driven manipulation in location-reward association challenged by newer studies?</t>
+  </si>
+  <si>
+    <t>Did researchers find a significant location-reward effect even when participants were not actively searching for high-reward locations?</t>
+  </si>
+  <si>
+    <t>How do the health mediators' work increase their self-esteem and social status in relation to the Hungarian Primary Care Model Programme?</t>
+  </si>
+  <si>
+    <t>Are there studies to suggest that there are potential downsides to leader empathy in the context of giving negative feedback?</t>
+  </si>
+  <si>
+    <t>There might be no significant differences in conscientious intelligence sub-dimensions between first and fourth-year nursing students because studies found that factors such as willingness to choose nursing as a profession, gender (female), and not perceiving nursing as solely a means to earn money were more influential in determining conscientious intelligence scores than academic year level.</t>
+  </si>
+  <si>
+    <t>Space topological cognition adds the following to the navigation model:
+Understanding of spatial relationships: This helps the model grasp how places relate to each other.
+Flexible path planning and detour behavior: Enables the model to find alternative routes or create detours when the original path is blocked.
+Adaptability: Allows the model to generalize its navigation skills to new or slightly changed environments.</t>
+  </si>
+  <si>
+    <t>What does the concept of space topological cognition add to the navigation model?</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>Clinicians can improve their communication by understanding patients' values, treating them with respect, acknowledging emotional and social realities, recognizing implicit biases, being mindful of language around topics like weight and food, and using verbal and nonverbal approaches to convey empathic concern.</t>
+  </si>
+  <si>
+    <t>How can emotionally intelligent leaders use their emotional intelligence to specifically address the challenges of stress, exhaustion, and the risk of moral injury brought on by the COVID-19 pandemic?</t>
+  </si>
+  <si>
+    <t>Emotionally intelligent leaders can use emotional intelligence to specifically address the challenges of stress, exhaustion, and the risk of moral injury brought on by the COVID-19 pandemic by supporting their teams, fostering effective personal relationships, and directing them towards common goals while demonstrating sensitivity to their psychological health and well-being.</t>
+  </si>
+  <si>
+    <t>What does the concept of space topological cognition add to a target driven visual navigation model?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is Delay Discounting (DD)? </t>
+  </si>
+  <si>
+    <t>Delay discounting (DD) refers to how rapidly an individual devalues goods based on delays to receipt.</t>
+  </si>
+  <si>
+    <t>Children with less severe ASD symptoms and with higher I.Q. are also diagnosed at later ages.</t>
+  </si>
+  <si>
+    <t>Are children with less severe ASD symptoms and with higher I.Q. diagnosed at earlier or later ages?</t>
+  </si>
+  <si>
+    <t>What emerging field of study addresses the limitations of traditional safety ergonomics in the era of big data with the aim to enhance both safety and cleaner production practices?</t>
+  </si>
+  <si>
+    <t>Examining the relationship between cognitive intelligence (CI), emotional intelligence (EI), and religiosity, what implications could this have for understanding the complexity of belief systems and differences in religious affiliation?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The negative association between cognitive intelligence (CI) and religiosity has been widely studied and is now well documented. In contrast, the role of emotional intelligence (EI) in this context has been poorly investigated thus far. Some available data indicate that EI, unlike CI, correlates positively with religiosity. To date, however, no study has explored the relationship between religiosity and both intelligences simultaneously. In current studies (Ns = 301 and 200), we examined the interplay between all three constructs. The results showed that CI was positively correlated with ability EI and negatively with some measures of religiosity. EI, on the other hand, revealed no direct, significant relationship with religiosity. However, when combined into a single regression model with CI, EI became a significant positive predictor of religiosity. Moreover, Study 2 revealed that the link between EI and religiosity was mediated by empathy. Interestingly, we also found a reciprocal suppression between CI and EI, since both predictors increased their influence on religiosity when analyzed together. Although the suppression was present in both studies, it was observed for different religiosity measures in each case, indicating that this effect is probably dependent on various factors, such as sample structure or type of religiosity.
+Keywords: Belief; Cognitive intelligence; Emotional intelligence; Empathy; Religiosity.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The relationship between cognitive and emotional intelligence and religiosity is multifaceted. While cognitive intelligence shows a negative association with some measures of religiosity, emotional intelligence does not exhibit a direct relationship. However, when considered together, emotional intelligence becomes a significant predictor of religiosity, mediated by empathy. The presence of reciprocal suppression between cognitive and emotional intelligence highlights the intricate dynamics involved in understanding how different types of intelligence influence religious beliefs. </t>
+  </si>
+  <si>
+    <t>How do individual differences in information processing speed correlate to general intelligence?</t>
+  </si>
+  <si>
+    <t>Individual differences in the speed of information processing have been hypothesized to give rise to individual differences in general intelligence. Consistent with this hypothesis, reaction times (RTs) and latencies of event-related potential have been shown to be moderately associated with intelligence. These associations have been explained either in terms of individual differences in some brain-wide property such as myelination, the speed of neural oscillations, or white-matter tract integrity, or in terms of individual differences in specific processes such as the signal-to-noise ratio in evidence accumulation, executive control, or the cholinergic system. Here we show in a sample of 122 participants, who completed a battery of RT tasks at 2 laboratory sessions while an EEG was recorded, that more intelligent individuals have a higher speed of higher-order information processing that explains about 80% of the variance in general intelligence. Our results do not support the notion that individuals with higher levels of general intelligence show advantages in some brain-wide property. Instead, they suggest that more intelligent individuals benefit from a more efficient transmission of information from frontal attention and working memory processes to temporal-parietal processes of memory storage. (PsycINFO Database Record</t>
+  </si>
+  <si>
+    <t>Individual differences in information processing speed are positively correlated with general intelligence, with more intelligent individuals demonstrating faster higher-order information processing that explains about 80% of the variance in general intelligence. This relationship is mediated by the efficiency of information transmission from frontal attention and working memory processes to temporal-parietal memory storage areas.</t>
+  </si>
+  <si>
+    <t>The strong relation between fluid reasoning (Gf) and working memory (WM) is well established. Gf depends on WM to hold necessary information in a span of awareness until the reasoning task is completed. The influence of time constraints on the Gf-WM relation indicates that the abilities to control attention and inhibit interference may be the underlying traits that account for the Gf-WM relation. Neuroanatomy also explains the interrelations among these cognitive processes. Neuroimaging (fMRI) studies have confirmed that the same regions of the prefrontal cortex (PFC) are active during Gf and WM functioning. The dorsolateral prefrontal cortex (dPFC) is also a critical structure for attention functions and inhibition.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How is fluid reasoning (Gf) related with working memory (WM)? </t>
+  </si>
+  <si>
+    <t>There is a strong relation between fluid reasoning (Gf) and working memory (WM). Gf depends on WM to hold necessary information in a span of awareness until the reasoning task is completed. The influence of time constraints on the Gf-WM relation indicates that the abilities to control attention and inhibit interference may be the underlying traits that account for the Gf-WM relation.</t>
+  </si>
+  <si>
+    <t>The quality of decision and assessment of risk are key determinants of successful sport performance. Athletes differ fundamentally in their decision-making ability according to their athletic expertise level. Moreover, given the influence of emotions on decision-making, it is likely that a trait reflecting emotional functioning, trait emotional intelligence, may also influence decision-making. Therefore, the aim of this research was to investigate the respective contribution of athletic expertise and trait emotional intelligence to non-athletic decision-making. In total, 269 participants aged between 18 and 26 years with a range of athletic experience i.e. none (n = 71), novice (n = 54), amateur (n = 55), elite (n = 45) and super-elite (n = 44), completed the Emotional Intelligence Scale and the Cambridge Gambling Task. Regression modelling indicated a significant positive relationship of athletic expertise and trait emotional intelligence with the quality of decision-making, and a negative relationship with deliberation time and risk-taking. Cognitive skills transfer may explain the higher decision-making scores associated with higher athletic expertise, while individuals with higher trait emotional intelligence may anticipate better the emotional consequences linked with a gambling task, which may help individuals make better decisions and take less risks.</t>
+  </si>
+  <si>
+    <t>Tell me about the the effect of athletic expertise and trait emotional intelligence on decision-making</t>
+  </si>
+  <si>
+    <t>Research indicates a significant positive relationship of athletic expertise and trait emotional intelligence with the quality of decision-making, and a negative relationship with deliberation time and risk-taking. Cognitive skills transfer may explain the higher decision-making scores associated with higher athletic expertise, while individuals with higher trait emotional intelligence may anticipate better the emotional consequences linked with a gambling task, which may help individuals make better decisions and take less risks.</t>
+  </si>
+  <si>
+    <t>Are addictions associated with Emotional Intelligence deficits?</t>
+  </si>
+  <si>
+    <t>Yes, addictions are associated with EI deficits, compared to controls. However, aspects such as the small number of addictive disorders analyzed, methodological issues related to instruments for assessment of IE and the lack of follow-up remain significant limitations.</t>
+  </si>
+  <si>
+    <t>Introduction: Emotional intelligence (EI) has been defined as the ability to perceive, understand, use and manage emotions. Studying EI could potentially be useful in understanding addictive behaviors as well as for designing and planning interventions.
+Objectives: To conduct a critical review on EI impairment in addiction disorders.
+Methods: MEDLINE/PubMed, Google Scholar, Cochrane, LILACS, and SciELO databases were searched. Articles that used the standardized Mayer-Salovey-Caruso Emotional Intelligence Test (MSCEIT) instrument to assess EI in people with addictions and healthy controls were selected for the review.
+Results: We selected seven articles assessing EI and its associations with addiction disorders, mainly alcohol abuse and cocaine dependence. Most studies reported that individuals with addiction disorders had worse EI scores when compared to controls.
+Conclusion: Overall, the studies reviewed demonstrated that addictions are associated with EI deficits, compared to controls. However, aspects such as the small number of addictive disorders analyzed, methodological issues related to instruments for assessment of IE and the lack of follow-up remain significant limitations.</t>
+  </si>
+  <si>
+    <t>Does emotional intelligence (EI) have a significant correlation with neuroticism, tension, and anxiety among flight cadets undergoing simulated flight training?</t>
+  </si>
+  <si>
+    <t>Yes, emotional intelligence (EI) was significantly correlated with neuroticism, tension and anxiety. Emotional intelligence may directly or indirectly affect simulated flight performance and tension plays an important mediating role.</t>
+  </si>
+  <si>
+    <t>BACKGROUND: Flight cadets' emotion is a factor of great importance to flight training. So it is of profound significance to address how emotional factors affect flight training performance. The present study aimed to investigate the relationship between emotional intelligence (EI) and simulated flight performance (SFP), and explore the mechanism of emotional state as a mediator in the effect of EI on SFP.METHODS: Ninety undergraduates took part in the study. EI (Wong and Law Emotional Intelligence Scale), neuroticism (Eysenck Personality Questionnaire Revised), anxiety (State Anxiety Inventory), and tension (Profile of Mood States) were collected. Conducted were 9 h of simulated flight training in a simulator of the Type 6 Primary Trainer. The Delphi Experts Grading Method was used to assess students' SFP. Mediation effect of emotional state was explored using regression analysis.RESULTS: EI was significantly correlated with neuroticism (r = -0.31), tension (r = -0.31), and anxiety (r = -0.31), respectively. Multiple mediation effects showed that emotional state mediated the association between EI and SFP. Tension especially mediated the associations between the Self Emotion Appraisals and Regulation of Emotion dimensions of EI and SFP. However, the Use of Emotion dimension of EI had a direct negative effect on SFP without the mediating role of emotional state.DISCUSSION: The findings indicated that EI was significantly correlated with emotional state (neuroticism, tension, and anxiety). EI may directly or indirectly affect SFP and tension played an important mediating role. Implications for the promotion of EI and emotional state to enhance performance in real flight training are discussed.Dai J, Wang H, Yang L, Wen Z. Emotional intelligence and emotional state effects on simulated flight performance. Aerosp Med Hum Perform. 2019; 90(2):101-108.</t>
   </si>
 </sst>
 </file>
@@ -1211,12 +1309,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1232,9 +1336,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1552,9 +1657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C3B921-A260-8D4A-9BAD-EC588CEF4C8E}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1567,753 +1670,793 @@
     <col min="7" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="C1" t="s">
+        <v>331</v>
+      </c>
+      <c r="D1" t="s">
+        <v>330</v>
+      </c>
+      <c r="E1" t="s">
+        <v>329</v>
+      </c>
+      <c r="F1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D2" t="s">
+        <v>327</v>
+      </c>
+      <c r="E2"/>
+      <c r="F2"/>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>326</v>
+      </c>
+      <c r="B3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C3" t="s">
+        <v>324</v>
+      </c>
+      <c r="D3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E3"/>
+      <c r="F3"/>
+    </row>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>317</v>
+      </c>
+      <c r="B4" t="s">
+        <v>322</v>
+      </c>
+      <c r="C4" t="s">
+        <v>321</v>
+      </c>
+      <c r="D4" t="s">
+        <v>320</v>
+      </c>
+      <c r="E4" t="s">
+        <v>319</v>
+      </c>
+      <c r="F4" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>317</v>
+      </c>
+      <c r="B5" t="s">
+        <v>316</v>
+      </c>
+      <c r="C5" t="s">
+        <v>315</v>
+      </c>
+      <c r="D5" t="s">
+        <v>314</v>
+      </c>
+      <c r="E5" t="s">
+        <v>313</v>
+      </c>
+      <c r="F5" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>309</v>
+      </c>
+      <c r="B6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C6" t="s">
+        <v>172</v>
+      </c>
+      <c r="D6" t="s">
+        <v>311</v>
+      </c>
+      <c r="E6" t="s">
+        <v>170</v>
+      </c>
+      <c r="F6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>309</v>
+      </c>
+      <c r="B7" t="s">
+        <v>308</v>
+      </c>
+      <c r="C7" t="s">
+        <v>307</v>
+      </c>
+      <c r="D7" t="s">
+        <v>306</v>
+      </c>
+      <c r="E7" t="s">
+        <v>305</v>
+      </c>
+      <c r="F7" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>298</v>
+      </c>
+      <c r="B8" t="s">
+        <v>303</v>
+      </c>
+      <c r="C8" t="s">
+        <v>302</v>
+      </c>
+      <c r="D8" t="s">
+        <v>301</v>
+      </c>
+      <c r="E8" t="s">
+        <v>300</v>
+      </c>
+      <c r="F8" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>298</v>
+      </c>
+      <c r="B9" t="s">
+        <v>297</v>
+      </c>
+      <c r="C9" t="s">
+        <v>296</v>
+      </c>
+      <c r="D9" t="s">
+        <v>295</v>
+      </c>
+      <c r="E9" t="s">
+        <v>294</v>
+      </c>
+      <c r="F9" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>287</v>
+      </c>
+      <c r="B10" t="s">
+        <v>292</v>
+      </c>
+      <c r="C10" t="s">
+        <v>291</v>
+      </c>
+      <c r="D10" t="s">
+        <v>290</v>
+      </c>
+      <c r="E10" t="s">
+        <v>289</v>
+      </c>
+      <c r="F10" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>287</v>
+      </c>
+      <c r="B11" t="s">
+        <v>286</v>
+      </c>
+      <c r="C11" t="s">
+        <v>285</v>
+      </c>
+      <c r="D11" t="s">
+        <v>284</v>
+      </c>
+      <c r="E11" t="s">
+        <v>283</v>
+      </c>
+      <c r="F11" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>280</v>
+      </c>
+      <c r="B12" t="s">
+        <v>167</v>
+      </c>
+      <c r="C12" t="s">
+        <v>166</v>
+      </c>
+      <c r="D12" t="s">
+        <v>281</v>
+      </c>
+      <c r="E12" t="s">
+        <v>164</v>
+      </c>
+      <c r="F12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>280</v>
+      </c>
+      <c r="B13" t="s">
+        <v>279</v>
+      </c>
+      <c r="C13" t="s">
+        <v>278</v>
+      </c>
+      <c r="D13" t="s">
+        <v>277</v>
+      </c>
+      <c r="E13" t="s">
+        <v>276</v>
+      </c>
+      <c r="F13" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>269</v>
+      </c>
+      <c r="B14" t="s">
+        <v>274</v>
+      </c>
+      <c r="C14" t="s">
+        <v>273</v>
+      </c>
+      <c r="D14" t="s">
+        <v>272</v>
+      </c>
+      <c r="E14" t="s">
+        <v>271</v>
+      </c>
+      <c r="F14" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>269</v>
+      </c>
+      <c r="B15" t="s">
+        <v>268</v>
+      </c>
+      <c r="C15" t="s">
+        <v>267</v>
+      </c>
+      <c r="D15" t="s">
+        <v>266</v>
+      </c>
+      <c r="E15" t="s">
+        <v>265</v>
+      </c>
+      <c r="F15" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>260</v>
+      </c>
+      <c r="B16" t="s">
+        <v>263</v>
+      </c>
+      <c r="C16" t="s">
+        <v>262</v>
+      </c>
+      <c r="D16" t="s">
+        <v>261</v>
+      </c>
+      <c r="E16"/>
+      <c r="F16"/>
+    </row>
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>260</v>
+      </c>
+      <c r="B17" t="s">
+        <v>259</v>
+      </c>
+      <c r="C17" t="s">
+        <v>258</v>
+      </c>
+      <c r="D17" t="s">
+        <v>257</v>
+      </c>
+      <c r="E17"/>
+      <c r="F17"/>
+    </row>
+    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>251</v>
+      </c>
+      <c r="B18" t="s">
+        <v>256</v>
+      </c>
+      <c r="C18" t="s">
+        <v>255</v>
+      </c>
+      <c r="D18" t="s">
+        <v>254</v>
+      </c>
+      <c r="E18" t="s">
+        <v>253</v>
+      </c>
+      <c r="F18" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>251</v>
+      </c>
+      <c r="B19" t="s">
+        <v>250</v>
+      </c>
+      <c r="C19" t="s">
+        <v>247</v>
+      </c>
+      <c r="D19" t="s">
+        <v>249</v>
+      </c>
+      <c r="E19" t="s">
+        <v>248</v>
+      </c>
+      <c r="F19" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>241</v>
+      </c>
+      <c r="B20" t="s">
+        <v>246</v>
+      </c>
+      <c r="C20" t="s">
+        <v>245</v>
+      </c>
+      <c r="D20" t="s">
+        <v>244</v>
+      </c>
+      <c r="E20" t="s">
+        <v>243</v>
+      </c>
+      <c r="F20" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>241</v>
+      </c>
+      <c r="B21" t="s">
+        <v>240</v>
+      </c>
+      <c r="C21" t="s">
+        <v>218</v>
+      </c>
+      <c r="D21" t="s">
+        <v>239</v>
+      </c>
+      <c r="E21" t="s">
+        <v>238</v>
+      </c>
+      <c r="F21" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>231</v>
+      </c>
+      <c r="B22" t="s">
+        <v>236</v>
+      </c>
+      <c r="C22" t="s">
+        <v>235</v>
+      </c>
+      <c r="D22" t="s">
+        <v>234</v>
+      </c>
+      <c r="E22" t="s">
+        <v>233</v>
+      </c>
+      <c r="F22" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>231</v>
+      </c>
+      <c r="B23" t="s">
+        <v>230</v>
+      </c>
+      <c r="C23" t="s">
+        <v>229</v>
+      </c>
+      <c r="D23" t="s">
+        <v>228</v>
+      </c>
+      <c r="E23" t="s">
+        <v>227</v>
+      </c>
+      <c r="F23" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>220</v>
+      </c>
+      <c r="B24" t="s">
+        <v>225</v>
+      </c>
+      <c r="C24" t="s">
+        <v>224</v>
+      </c>
+      <c r="D24" t="s">
+        <v>223</v>
+      </c>
+      <c r="E24" t="s">
+        <v>222</v>
+      </c>
+      <c r="F24" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>220</v>
+      </c>
+      <c r="B25" t="s">
+        <v>219</v>
+      </c>
+      <c r="C25" t="s">
+        <v>218</v>
+      </c>
+      <c r="D25" t="s">
+        <v>217</v>
+      </c>
+      <c r="E25"/>
+      <c r="F25"/>
+    </row>
+    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>211</v>
+      </c>
+      <c r="B26" t="s">
+        <v>216</v>
+      </c>
+      <c r="C26" t="s">
+        <v>215</v>
+      </c>
+      <c r="D26" t="s">
+        <v>214</v>
+      </c>
+      <c r="E26" t="s">
+        <v>213</v>
+      </c>
+      <c r="F26" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>211</v>
+      </c>
+      <c r="B27" t="s">
+        <v>210</v>
+      </c>
+      <c r="C27" t="s">
+        <v>209</v>
+      </c>
+      <c r="D27" t="s">
+        <v>208</v>
+      </c>
+      <c r="E27" t="s">
+        <v>207</v>
+      </c>
+      <c r="F27" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>200</v>
+      </c>
+      <c r="B28" t="s">
+        <v>205</v>
+      </c>
+      <c r="C28" t="s">
+        <v>204</v>
+      </c>
+      <c r="D28" t="s">
+        <v>203</v>
+      </c>
+      <c r="E28" t="s">
+        <v>202</v>
+      </c>
+      <c r="F28" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>200</v>
+      </c>
+      <c r="B29" t="s">
+        <v>199</v>
+      </c>
+      <c r="C29" t="s">
+        <v>198</v>
+      </c>
+      <c r="D29" t="s">
+        <v>197</v>
+      </c>
+      <c r="E29" t="s">
+        <v>196</v>
+      </c>
+      <c r="F29" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>189</v>
+      </c>
+      <c r="B30" t="s">
+        <v>194</v>
+      </c>
+      <c r="C30" t="s">
+        <v>193</v>
+      </c>
+      <c r="D30" t="s">
+        <v>192</v>
+      </c>
+      <c r="E30" t="s">
+        <v>191</v>
+      </c>
+      <c r="F30" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>189</v>
+      </c>
+      <c r="B31" t="s">
+        <v>188</v>
+      </c>
+      <c r="C31" t="s">
+        <v>187</v>
+      </c>
+      <c r="D31" t="s">
+        <v>186</v>
+      </c>
+      <c r="E31" t="s">
+        <v>181</v>
+      </c>
+      <c r="F31" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>179</v>
+      </c>
+      <c r="B32" t="s">
+        <v>184</v>
+      </c>
+      <c r="C32" t="s">
+        <v>183</v>
+      </c>
+      <c r="D32" t="s">
+        <v>182</v>
+      </c>
+      <c r="E32" t="s">
+        <v>181</v>
+      </c>
+      <c r="F32" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>179</v>
+      </c>
+      <c r="B33" t="s">
+        <v>178</v>
+      </c>
+      <c r="C33" t="s">
+        <v>177</v>
+      </c>
+      <c r="D33" t="s">
+        <v>176</v>
+      </c>
+      <c r="E33" t="s">
+        <v>175</v>
+      </c>
+      <c r="F33" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>168</v>
+      </c>
+      <c r="B34" t="s">
+        <v>173</v>
+      </c>
+      <c r="C34" t="s">
+        <v>172</v>
+      </c>
+      <c r="D34" t="s">
+        <v>171</v>
+      </c>
+      <c r="E34" t="s">
+        <v>170</v>
+      </c>
+      <c r="F34" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>168</v>
+      </c>
+      <c r="B35" t="s">
+        <v>167</v>
+      </c>
+      <c r="C35" t="s">
+        <v>166</v>
+      </c>
+      <c r="D35" t="s">
+        <v>165</v>
+      </c>
+      <c r="E35" t="s">
+        <v>164</v>
+      </c>
+      <c r="F35" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>157</v>
+      </c>
+      <c r="B36" t="s">
+        <v>162</v>
+      </c>
+      <c r="C36" t="s">
+        <v>161</v>
+      </c>
+      <c r="D36" t="s">
+        <v>160</v>
+      </c>
+      <c r="E36" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="F36" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>157</v>
+      </c>
+      <c r="B37" t="s">
+        <v>156</v>
+      </c>
+      <c r="C37" t="s">
+        <v>155</v>
+      </c>
+      <c r="D37" t="s">
+        <v>154</v>
+      </c>
+      <c r="E37" t="s">
+        <v>153</v>
+      </c>
+      <c r="F37" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>160</v>
-      </c>
+      <c r="B38" t="s">
+        <v>370</v>
+      </c>
+      <c r="C38" t="s">
+        <v>371</v>
+      </c>
+      <c r="D38"/>
+      <c r="E38">
+        <v>30994781</v>
+      </c>
+      <c r="F38" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>280</v>
+      </c>
+      <c r="B39" t="s">
+        <v>373</v>
+      </c>
+      <c r="C39" t="s">
+        <v>374</v>
+      </c>
+      <c r="D39"/>
+      <c r="E39">
+        <v>30670119</v>
+      </c>
+      <c r="F39" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>148</v>
+      </c>
+      <c r="B40" t="s">
+        <v>151</v>
+      </c>
+      <c r="C40" t="s">
+        <v>150</v>
+      </c>
+      <c r="D40" t="s">
+        <v>149</v>
+      </c>
+      <c r="E40"/>
+      <c r="F40"/>
+    </row>
+    <row r="41" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>148</v>
+      </c>
+      <c r="B41" t="s">
+        <v>147</v>
+      </c>
+      <c r="C41" t="s">
+        <v>146</v>
+      </c>
+      <c r="D41" t="s">
+        <v>145</v>
+      </c>
+      <c r="E41"/>
+      <c r="F41"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2324,15 +2467,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ECB6FD1-CDBE-694D-8700-2DD50D52B540}">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="48.83203125" customWidth="1"/>
-    <col min="2" max="2" width="50.5" customWidth="1"/>
-    <col min="3" max="3" width="46.1640625" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" customWidth="1"/>
+    <col min="4" max="4" width="255.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -2343,10 +2487,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="D1" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2360,35 +2504,35 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>345</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>99</v>
+      <c r="D3" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
-        <v>100</v>
+      <c r="D4" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2396,307 +2540,307 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>332</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
-        <v>102</v>
+      <c r="D6" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D8" t="s">
-        <v>104</v>
+      <c r="C8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
       <c r="D10" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>333</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>334</v>
+      </c>
+      <c r="C15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" t="s">
-        <v>112</v>
+      <c r="C16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="B19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" t="s">
-        <v>116</v>
+      <c r="B20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D21" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" t="s">
         <v>39</v>
       </c>
-      <c r="C22" t="s">
-        <v>42</v>
-      </c>
       <c r="D22" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B23" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" t="s">
-        <v>120</v>
+      <c r="C24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D25" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" t="s">
         <v>47</v>
       </c>
-      <c r="B26" t="s">
-        <v>50</v>
-      </c>
       <c r="C26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D26" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -2704,13 +2848,13 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D27" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -2718,13 +2862,13 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D28" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -2732,13 +2876,13 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>335</v>
       </c>
       <c r="C29" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D29" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -2746,13 +2890,13 @@
         <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D30" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -2760,27 +2904,27 @@
         <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C31" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D31" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D32" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -2788,13 +2932,13 @@
         <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C33" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D33" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -2802,13 +2946,13 @@
         <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C34" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D34" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -2816,167 +2960,167 @@
         <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>62</v>
+        <v>336</v>
       </c>
       <c r="C35" t="s">
-        <v>59</v>
+        <v>337</v>
       </c>
       <c r="D35" t="s">
-        <v>131</v>
+        <v>338</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C36" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D36" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B37" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C37" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D37" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B38" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C38" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D38" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" t="s">
+        <v>339</v>
+      </c>
+      <c r="C39" t="s">
+        <v>58</v>
+      </c>
+      <c r="D39" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B39" t="s">
-        <v>67</v>
-      </c>
-      <c r="C39" t="s">
-        <v>63</v>
-      </c>
-      <c r="D39" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>30</v>
-      </c>
-      <c r="B40" t="s">
-        <v>68</v>
-      </c>
-      <c r="C40" t="s">
-        <v>63</v>
-      </c>
-      <c r="D40" t="s">
-        <v>136</v>
+      <c r="B40" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>22</v>
-      </c>
-      <c r="B41" t="s">
-        <v>70</v>
-      </c>
-      <c r="C41" t="s">
-        <v>69</v>
-      </c>
-      <c r="D41" t="s">
-        <v>137</v>
+      <c r="A41" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B42" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C42" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D42" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B43" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C43" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D43" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B44" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C44" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D44" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>47</v>
-      </c>
-      <c r="B45" t="s">
-        <v>75</v>
-      </c>
-      <c r="C45" t="s">
-        <v>74</v>
-      </c>
-      <c r="D45" t="s">
-        <v>141</v>
+      <c r="A45" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C46" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D46" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -2984,13 +3128,13 @@
         <v>3</v>
       </c>
       <c r="B47" t="s">
-        <v>78</v>
+        <v>341</v>
       </c>
       <c r="C47" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D47" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -2998,13 +3142,13 @@
         <v>6</v>
       </c>
       <c r="B48" t="s">
-        <v>79</v>
+        <v>342</v>
       </c>
       <c r="C48" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D48" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -3012,139 +3156,139 @@
         <v>8</v>
       </c>
       <c r="B49" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C49" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D49" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>22</v>
-      </c>
-      <c r="B50" t="s">
-        <v>82</v>
-      </c>
-      <c r="C50" t="s">
-        <v>81</v>
-      </c>
-      <c r="D50" t="s">
-        <v>146</v>
+      <c r="A50" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B51" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C51" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D51" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B52" t="s">
-        <v>84</v>
+        <v>343</v>
       </c>
       <c r="C52" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D52" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B53" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C53" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D53" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B54" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C54" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D54" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B55" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C55" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D55" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B56" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="C56" t="s">
+        <v>71</v>
+      </c>
+      <c r="D56" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D56" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>3</v>
-      </c>
-      <c r="B57" t="s">
-        <v>90</v>
-      </c>
-      <c r="C57" t="s">
-        <v>92</v>
-      </c>
-      <c r="D57" t="s">
-        <v>153</v>
+      <c r="D57" s="2" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B58" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C58" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="D58" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -3152,13 +3296,13 @@
         <v>3</v>
       </c>
       <c r="B59" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="C59" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="D59" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -3166,27 +3310,340 @@
         <v>6</v>
       </c>
       <c r="B60" t="s">
-        <v>95</v>
+        <v>344</v>
       </c>
       <c r="C60" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="D60" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+      <c r="A61" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B61" t="s">
-        <v>96</v>
-      </c>
-      <c r="C61" t="s">
-        <v>97</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="B61" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F822382-AE75-4447-AC6A-1AB56E8F35E1}">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView zoomScale="125" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="47.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="189.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>317</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>280</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>269</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>269</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>269</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>251</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>269</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B10" t="s">
+        <v>340</v>
+      </c>
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>269</v>
+      </c>
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>251</v>
+      </c>
+      <c r="B12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>251</v>
+      </c>
+      <c r="B13" t="s">
+        <v>350</v>
+      </c>
+      <c r="C13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>269</v>
+      </c>
+      <c r="B14" t="s">
+        <v>352</v>
+      </c>
+      <c r="C14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>269</v>
+      </c>
+      <c r="B15" t="s">
+        <v>353</v>
+      </c>
+      <c r="C15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" t="s">
+        <v>356</v>
+      </c>
+      <c r="C16" t="s">
+        <v>337</v>
+      </c>
+      <c r="D16" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>269</v>
+      </c>
+      <c r="B17" t="s">
+        <v>357</v>
+      </c>
+      <c r="C17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>231</v>
+      </c>
+      <c r="B18" t="s">
+        <v>358</v>
+      </c>
+      <c r="C18" t="s">
+        <v>359</v>
+      </c>
+      <c r="D18" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>269</v>
+      </c>
+      <c r="B19" t="s">
+        <v>361</v>
+      </c>
+      <c r="C19" t="s">
+        <v>362</v>
+      </c>
+      <c r="D19" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>269</v>
+      </c>
+      <c r="B20" t="s">
+        <v>365</v>
+      </c>
+      <c r="C20" t="s">
+        <v>364</v>
+      </c>
+      <c r="D20" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>157</v>
+      </c>
+      <c r="B21" t="s">
+        <v>368</v>
+      </c>
+      <c r="C21" t="s">
+        <v>367</v>
+      </c>
+      <c r="D21" t="s">
+        <v>369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated question types for evaluation for 60 questions
</commit_message>
<xml_diff>
--- a/kedronlp/notebooks/Evaluation.xlsx
+++ b/kedronlp/notebooks/Evaluation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arjan/Bachelor/NLP with Transformers/pubMedNLP/kedronlp/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255BEEDB-53A9-F447-B260-630D2CD314EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF36B35-CB9B-BA4E-94CD-BC6C04795971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16120" xr2:uid="{3AC1803B-D431-F74E-BDCB-3D80AD30DE94}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="385">
   <si>
     <t>Question Type</t>
   </si>
@@ -1287,6 +1287,33 @@
   </si>
   <si>
     <t>BACKGROUND: Flight cadets' emotion is a factor of great importance to flight training. So it is of profound significance to address how emotional factors affect flight training performance. The present study aimed to investigate the relationship between emotional intelligence (EI) and simulated flight performance (SFP), and explore the mechanism of emotional state as a mediator in the effect of EI on SFP.METHODS: Ninety undergraduates took part in the study. EI (Wong and Law Emotional Intelligence Scale), neuroticism (Eysenck Personality Questionnaire Revised), anxiety (State Anxiety Inventory), and tension (Profile of Mood States) were collected. Conducted were 9 h of simulated flight training in a simulator of the Type 6 Primary Trainer. The Delphi Experts Grading Method was used to assess students' SFP. Mediation effect of emotional state was explored using regression analysis.RESULTS: EI was significantly correlated with neuroticism (r = -0.31), tension (r = -0.31), and anxiety (r = -0.31), respectively. Multiple mediation effects showed that emotional state mediated the association between EI and SFP. Tension especially mediated the associations between the Self Emotion Appraisals and Regulation of Emotion dimensions of EI and SFP. However, the Use of Emotion dimension of EI had a direct negative effect on SFP without the mediating role of emotional state.DISCUSSION: The findings indicated that EI was significantly correlated with emotional state (neuroticism, tension, and anxiety). EI may directly or indirectly affect SFP and tension played an important mediating role. Implications for the promotion of EI and emotional state to enhance performance in real flight training are discussed.Dai J, Wang H, Yang L, Wen Z. Emotional intelligence and emotional state effects on simulated flight performance. Aerosp Med Hum Perform. 2019; 90(2):101-108.</t>
+  </si>
+  <si>
+    <t>factoid</t>
+  </si>
+  <si>
+    <t>comparative</t>
+  </si>
+  <si>
+    <t>yes/no</t>
+  </si>
+  <si>
+    <t>hypothetical</t>
+  </si>
+  <si>
+    <t>descriptive</t>
+  </si>
+  <si>
+    <t>open-ended</t>
+  </si>
+  <si>
+    <t>Question Type Detailed</t>
+  </si>
+  <si>
+    <t>multiple-choice</t>
+  </si>
+  <si>
+    <t>how</t>
   </si>
 </sst>
 </file>
@@ -1655,808 +1682,934 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C3B921-A260-8D4A-9BAD-EC588CEF4C8E}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="54.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="233.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="255.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="255.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="255.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="233.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="255.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="255.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>382</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>331</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>330</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>329</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B2" t="s">
         <v>326</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>328</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>324</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>327</v>
       </c>
-      <c r="E2"/>
       <c r="F2"/>
-    </row>
-    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>376</v>
+      </c>
+      <c r="B3" t="s">
         <v>326</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>325</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>324</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>323</v>
       </c>
-      <c r="E3"/>
       <c r="F3"/>
-    </row>
-    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>376</v>
+      </c>
+      <c r="B4" t="s">
         <v>317</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>322</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>321</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>320</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>319</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>376</v>
+      </c>
+      <c r="B5" t="s">
         <v>317</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>316</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>315</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>314</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>313</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>376</v>
+      </c>
+      <c r="B6" t="s">
         <v>309</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>173</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>172</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>311</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>170</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>380</v>
+      </c>
+      <c r="B7" t="s">
         <v>309</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>308</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>307</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>306</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>305</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>380</v>
+      </c>
+      <c r="B8" t="s">
         <v>298</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>303</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>302</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>301</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>300</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>376</v>
+      </c>
+      <c r="B9" t="s">
         <v>298</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>297</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>296</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>295</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>294</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>381</v>
+      </c>
+      <c r="B10" t="s">
         <v>287</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>292</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>291</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>290</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>289</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>377</v>
+      </c>
+      <c r="B11" t="s">
         <v>287</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>286</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>285</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>284</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>283</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>378</v>
+      </c>
+      <c r="B12" t="s">
         <v>280</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>167</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>166</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>281</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>164</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>378</v>
+      </c>
+      <c r="B13" t="s">
         <v>280</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>279</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>278</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>277</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>276</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>376</v>
+      </c>
+      <c r="B14" t="s">
         <v>269</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>274</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>273</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>272</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>271</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>376</v>
+      </c>
+      <c r="B15" t="s">
         <v>269</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>268</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>267</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>266</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>265</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>380</v>
+      </c>
+      <c r="B16" t="s">
         <v>260</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>263</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>262</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>261</v>
       </c>
-      <c r="E16"/>
       <c r="F16"/>
-    </row>
-    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G16"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>380</v>
+      </c>
+      <c r="B17" t="s">
         <v>260</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>259</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>258</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>257</v>
       </c>
-      <c r="E17"/>
       <c r="F17"/>
-    </row>
-    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G17"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>376</v>
+      </c>
+      <c r="B18" t="s">
         <v>251</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>256</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>255</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>254</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>253</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>376</v>
+      </c>
+      <c r="B19" t="s">
         <v>251</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>250</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>247</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>249</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>248</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>379</v>
+      </c>
+      <c r="B20" t="s">
         <v>241</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>246</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>245</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>244</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>243</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>379</v>
+      </c>
+      <c r="B21" t="s">
         <v>241</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>240</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>218</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>239</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>238</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>376</v>
+      </c>
+      <c r="B22" t="s">
         <v>231</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>236</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>235</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>234</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>233</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>376</v>
+      </c>
+      <c r="B23" t="s">
         <v>231</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>230</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>229</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>228</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>227</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>379</v>
+      </c>
+      <c r="B24" t="s">
         <v>220</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>225</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>224</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>223</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>222</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>379</v>
+      </c>
+      <c r="B25" t="s">
         <v>220</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>219</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>218</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>217</v>
       </c>
-      <c r="E25"/>
       <c r="F25"/>
-    </row>
-    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G25"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>376</v>
+      </c>
+      <c r="B26" t="s">
         <v>211</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>216</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>215</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>214</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>213</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>376</v>
+      </c>
+      <c r="B27" t="s">
         <v>211</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>210</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>209</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>208</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>207</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>376</v>
+      </c>
+      <c r="B28" t="s">
         <v>200</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>205</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>204</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>203</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>202</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>376</v>
+      </c>
+      <c r="B29" t="s">
         <v>200</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>199</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>198</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>197</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>196</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>376</v>
+      </c>
+      <c r="B30" t="s">
         <v>189</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>194</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>193</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>192</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>191</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>376</v>
+      </c>
+      <c r="B31" t="s">
         <v>189</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>188</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>187</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>186</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>181</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>381</v>
+      </c>
+      <c r="B32" t="s">
         <v>179</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>184</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>183</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>182</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>181</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>381</v>
+      </c>
+      <c r="B33" t="s">
         <v>179</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>178</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>177</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>176</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>175</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>376</v>
+      </c>
+      <c r="B34" t="s">
         <v>168</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>173</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>172</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>171</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>170</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>376</v>
+      </c>
+      <c r="B35" t="s">
         <v>168</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>167</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>166</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>165</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>164</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>380</v>
+      </c>
+      <c r="B36" t="s">
         <v>157</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>162</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>161</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>160</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>159</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>380</v>
+      </c>
+      <c r="B37" t="s">
         <v>157</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>156</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>155</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>154</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>153</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>378</v>
+      </c>
+      <c r="B38" t="s">
         <v>280</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>370</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>371</v>
       </c>
-      <c r="D38"/>
-      <c r="E38">
+      <c r="E38"/>
+      <c r="F38">
         <v>30994781</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>378</v>
+      </c>
+      <c r="B39" t="s">
         <v>280</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>373</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>374</v>
       </c>
-      <c r="D39"/>
-      <c r="E39">
+      <c r="E39"/>
+      <c r="F39">
         <v>30670119</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>377</v>
+      </c>
+      <c r="B40" t="s">
         <v>148</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>151</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>150</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>149</v>
       </c>
-      <c r="E40"/>
       <c r="F40"/>
-    </row>
-    <row r="41" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G40"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>377</v>
+      </c>
+      <c r="B41" t="s">
         <v>148</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>147</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>146</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>145</v>
       </c>
-      <c r="E41"/>
       <c r="F41"/>
+      <c r="G41"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3341,308 +3494,374 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F822382-AE75-4447-AC6A-1AB56E8F35E1}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="189.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="189.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="255.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>382</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>144</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>378</v>
+      </c>
+      <c r="B2" t="s">
         <v>280</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>383</v>
+      </c>
+      <c r="B3" t="s">
         <v>317</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>378</v>
+      </c>
+      <c r="B4" t="s">
         <v>280</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>376</v>
+      </c>
+      <c r="B5" t="s">
         <v>269</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>30</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>29</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>376</v>
+      </c>
+      <c r="B6" t="s">
         <v>269</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>33</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>29</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>384</v>
+      </c>
+      <c r="B7" t="s">
         <v>269</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>34</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>29</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>384</v>
+      </c>
+      <c r="B8" t="s">
         <v>251</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>384</v>
+      </c>
+      <c r="B9" t="s">
         <v>269</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>43</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>42</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>384</v>
+      </c>
+      <c r="B10" t="s">
         <v>269</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>340</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>58</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>376</v>
+      </c>
+      <c r="B11" t="s">
         <v>269</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>72</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>71</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>384</v>
+      </c>
+      <c r="B12" t="s">
         <v>251</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>79</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>81</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>384</v>
+      </c>
+      <c r="B13" t="s">
         <v>251</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>350</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>85</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>376</v>
+      </c>
+      <c r="B14" t="s">
         <v>269</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>352</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>62</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>376</v>
+      </c>
+      <c r="B15" t="s">
         <v>269</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>353</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>55</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>377</v>
+      </c>
+      <c r="B16" t="s">
         <v>148</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>356</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>337</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>376</v>
+      </c>
+      <c r="B17" t="s">
         <v>269</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>357</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>66</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>381</v>
+      </c>
+      <c r="B18" t="s">
         <v>231</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>358</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>359</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>381</v>
+      </c>
+      <c r="B19" t="s">
         <v>269</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>361</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>362</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>381</v>
+      </c>
+      <c r="B20" t="s">
         <v>269</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>365</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>364</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>380</v>
+      </c>
+      <c r="B21" t="s">
         <v>157</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>368</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>367</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>369</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added ChatGPT answers for first 60 questions from the dataset
</commit_message>
<xml_diff>
--- a/kedronlp/notebooks/Evaluation.xlsx
+++ b/kedronlp/notebooks/Evaluation.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arjan/Bachelor/NLP with Transformers/pubMedNLP/kedronlp/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF36B35-CB9B-BA4E-94CD-BC6C04795971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CEC233-AB14-7149-9086-5044A2A56DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16120" xr2:uid="{3AC1803B-D431-F74E-BDCB-3D80AD30DE94}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16120" activeTab="3" xr2:uid="{3AC1803B-D431-F74E-BDCB-3D80AD30DE94}"/>
   </bookViews>
   <sheets>
     <sheet name="Human" sheetId="3" r:id="rId1"/>
     <sheet name="Model" sheetId="1" r:id="rId2"/>
     <sheet name="Additional" sheetId="4" r:id="rId3"/>
+    <sheet name="ChatGPT" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="443">
   <si>
     <t>Question Type</t>
   </si>
@@ -1314,6 +1315,236 @@
   </si>
   <si>
     <t>how</t>
+  </si>
+  <si>
+    <t>GPTAnswer</t>
+  </si>
+  <si>
+    <t>The Golden Gate Bridge is approximately 746 feet (227 meters) tall.</t>
+  </si>
+  <si>
+    <t>The Eiffel Tower is located in Paris, France.</t>
+  </si>
+  <si>
+    <t>Predictors of nurses' attitudes towards communication can include factors such as:
+1. Training and education in communication skills.
+2. Work environment and organizational culture.
+3. Job satisfaction and stress levels.
+4. Interpersonal relationships with colleagues and patients.
+5. Personal communication styles and preferences.
+6. Perceived importance of effective communication in patient care.
+7. Exposure to communication barriers and challenges in the workplace.
+8. Support resources available for communication improvement.</t>
+  </si>
+  <si>
+    <t>Autism Spectrum Disorder (ASD) is characterized by challenges with social communication and interaction, as well as restricted and repetitive behaviors.</t>
+  </si>
+  <si>
+    <t>The TT100K dataset is a large-scale benchmark dataset for object detection and classification in traffic scenes. It contains over 100,000 images with annotated objects such as vehicles, pedestrians, and cyclists, captured from real-world traffic scenarios.</t>
+  </si>
+  <si>
+    <t>The full form of EHR is Electronic Health Records.
+Strengths of EHR:
+1. Improved accessibility and portability of patient records.
+2. Enhanced coordination of care among healthcare providers.
+3. Facilitation of clinical decision-making through access to comprehensive patient information.
+4. Reduction of medical errors through standardized documentation and alerts.
+5. Increased efficiency in healthcare delivery, such as faster retrieval of patient data.
+Limitations of EHR:
+1. Privacy and security concerns regarding patient data breaches.
+2. Potential for information overload, leading to cognitive overload for healthcare providers.
+3. Costs associated with implementation, maintenance, and training.
+4. Interoperability issues between different EHR systems, hindering data exchange.
+5. Risk of data inaccuracies and discrepancies due to human error or system malfunctions.</t>
+  </si>
+  <si>
+    <t>Network Neuroscience Theory (NNT): Proposes that general intelligence (g) arises from the overall organization of brain networks, rather than specific brain regions.
+Small-World Topology: Brains with higher g exhibit a balance of local clustering and long-range connections, optimizing efficiency and communication.
+Flexible Dynamics: High-g individuals demonstrate greater flexibility in how their brain networks reorganize in response to different tasks.
+Global Efficiency: Systems with high g show efficient information flow across the whole brain, supporting complex processing.</t>
+  </si>
+  <si>
+    <t>The best fit between brain traits and degrees of intelligence among mammals is reached by humans.</t>
+  </si>
+  <si>
+    <t>Intelligence is a complex, multifaceted trait that involves the ability to learn, understand, reason, adapt, and solve problems effectively. It encompasses various cognitive abilities such as memory, attention, language, creativity, and logical reasoning. Intelligence is not a single, fixed attribute but rather a combination of genetic predispositions, environmental factors, and individual experiences. It enables individuals to navigate and thrive in their environments by processing information, making decisions, and achieving goals.</t>
+  </si>
+  <si>
+    <t>The paper titled "What is theory of mind? A psychometric study of theory of mind and intelligence" was published first.</t>
+  </si>
+  <si>
+    <t>Yes, research suggests that forms of narcissism, such as grandiose and vulnerable narcissism, can be related to objective intelligence, although the nature of this relationship may vary.
+1. **Grandiose Narcissism**: Some studies have found a positive association between grandiose narcissism and intelligence. Grandiose narcissists often exhibit traits such as confidence, assertiveness, and a desire for admiration, which may be linked to higher levels of intelligence in certain domains, such as verbal intelligence or social intelligence.
+2. **Vulnerable Narcissism**: The relationship between vulnerable narcissism and intelligence is less clear and may depend on the specific traits and behaviors associated with this subtype. Vulnerable narcissists tend to have low self-esteem, hypersensitivity to criticism, and a tendency to avoid social situations. Their cognitive abilities may be impacted by factors such as anxiety or depression, which are commonly associated with vulnerable narcissism.
+Overall, while some studies suggest a positive association between certain aspects of narcissism and intelligence, other factors such as emotional regulation, social skills, and mental health may also influence this relationship. Additionally, the relationship between narcissism and intelligence is complex and may be moderated by various individual and situational factors.</t>
+  </si>
+  <si>
+    <t>In task-switching experiments, intellectually gifted children may indeed perform quicker than average children, but the specific results can vary based on the nature of the tasks and the individual characteristics of the participants.
+In some studies, intellectually gifted children have demonstrated faster reaction times and greater cognitive flexibility when switching between tasks compared to average children. This enhanced ability to adapt to changing task demands may allow gifted children to perform well in both mixed-trial blocks (where tasks are switched) and single-trial blocks (where tasks are repeated).
+However, it's important to note that individual differences in task performance can be influenced by various factors beyond intellectual giftedness, such as working memory capacity, attentional control, and motivation. Additionally, the specific methods and measures used in the experiment can also impact the results.
+Overall, while intellectually gifted children may exhibit advantages in certain cognitive tasks, the relationship between giftedness and task-switching performance can be nuanced and may depend on various contextual factors.</t>
+  </si>
+  <si>
+    <t>The Flynn Effect is the observed rise in average intelligence test scores over time. It challenges the idea of IQ as a fixed, innate trait, highlighting the role of environmental factors in shaping cognitive abilities.</t>
+  </si>
+  <si>
+    <t>Emotional exhaustion is a key component of burnout, often considered its core dimension. It refers to feelings of being emotionally drained, depleted, and overwhelmed by one's work or responsibilities. Emotional exhaustion can result from prolonged stress, excessive workload, lack of support, or a mismatch between personal values and job demands. In the context of burnout, emotional exhaustion is typically accompanied by feelings of cynicism and detachment from work (depersonalization) and a reduced sense of personal accomplishment. It is a significant predictor of overall burnout and can have negative consequences for both individual well-being and organizational effectiveness.</t>
+  </si>
+  <si>
+    <t>Different theories propose various types of intelligence, including:
+1. **Verbal-linguistic intelligence**: Strength in language-related skills such as reading, writing, speaking, and listening.
+2. **Logical-mathematical intelligence**: Ability to reason logically, think critically, and solve problems using numbers and abstract patterns.
+3. **Visual-spatial intelligence**: Capacity to perceive and manipulate visual information, understand spatial relationships, and solve problems using mental imagery.
+4. **Musical-rhythmic intelligence**: Aptitude for understanding and creating music, including pitch, rhythm, melody, and composition.
+5. **Bodily-kinesthetic intelligence**: Skill in using the body to perform tasks, such as sports, dance, or manual labor, and a heightened awareness of bodily movements and coordination.
+6. **Interpersonal intelligence**: Ability to understand and interact effectively with others, including empathy, social skills, and the capacity to perceive and respond to emotions in others.
+7. **Intrapersonal intelligence**: Insight into one's own thoughts, feelings, and motivations, and the ability to regulate emotions, set goals, and engage in self-reflection.
+8. **Naturalistic intelligence**: Sensitivity to and understanding of the natural world, including the ability to recognize and classify plants, animals, and natural phenomena.
+These types of intelligence are often conceptualized within Howard Gardner's theory of multiple intelligences, which suggests that individuals possess a unique combination of these intelligences, with varying strengths and weaknesses.</t>
+  </si>
+  <si>
+    <t>Here are some common abbreviations used in the field of intelligence in PubMed:
+1. IQ - Intelligence Quotient
+2. WAIS - Wechsler Adult Intelligence Scale
+3. WISC - Wechsler Intelligence Scale for Children
+4. Raven's - Raven's Progressive Matrices
+5. Cattell - Cattell's Culture Fair Intelligence Test
+6. PIQ - Performance IQ
+7. VIQ - Verbal IQ
+8. FSIQ - Full-Scale IQ
+9. GMA - General Mental Ability
+10. SAT - Scholastic Aptitude Test (though it's not exclusively an intelligence test, it's often used in research related to intelligence)
+These are just a few examples, and there may be more specific abbreviations depending on the context of the research.</t>
+  </si>
+  <si>
+    <t>Cephalopods evolved intelligence for survival advantages, including hunting, adapting to diverse environments, social interactions, tool use, and learning abilities.</t>
+  </si>
+  <si>
+    <t>Intelligence is associated with the stability of happiness because it enables individuals to navigate life's challenges more effectively, make informed decisions, and cope with setbacks. Additionally, intelligent individuals may have better problem-solving skills, stronger social support networks, and greater access to resources, all of which contribute to resilience and overall well-being over time.</t>
+  </si>
+  <si>
+    <t>Improved cognitive health, delayed cognitive decline, enhanced quality of life, potentially reduced healthcare costs, and public health initiatives promoting cognitive-supportive diets.</t>
+  </si>
+  <si>
+    <t>Optimized supply chain management, reduced costs, improved efficiency, and better decision-making.</t>
+  </si>
+  <si>
+    <t>Themes that emerged include improved patient outcomes, enhanced communication, better self-awareness among clinicians, and more effective interdisciplinary collaboration.</t>
+  </si>
+  <si>
+    <t>The study likely employed tools such as standardized intelligence tests (e.g., IQ tests), questionnaires or surveys to assess intrinsic motivation, and possibly qualitative methods such as interviews or observations to gather data on participants' behaviors and attitudes.</t>
+  </si>
+  <si>
+    <t>These names appear to be authors or researchers associated with a study or academic paper.</t>
+  </si>
+  <si>
+    <t>It seems like you've entered a random string of characters. How can I assist you further?</t>
+  </si>
+  <si>
+    <t>I couldn't find a paper with that exact title. It's possible that it's a newer publication or not indexed in the databases I have access to.</t>
+  </si>
+  <si>
+    <t>The neuroscience of empathy and compassion in pro-social behavior was published in 2012.</t>
+  </si>
+  <si>
+    <t>The Individuals with Disabilities Education Act (IDEA) is a law in the United States.</t>
+  </si>
+  <si>
+    <t>Fill in the blank: Impact of Artificial Intelligence on Regional Green Development under China's Environmental Decentralization System-Based on Spatial Durbin Model and Threshold Effect</t>
+  </si>
+  <si>
+    <t>International differences in student assessment and IQ test results can stem from socioeconomic disparities, cultural factors, educational policies, language diversity, test bias, sampling variations, and a mix of genetic and environmental influences.</t>
+  </si>
+  <si>
+    <t>Higher IQ scores are significantly associated with factors such as education level, socioeconomic status, parental education, genetic factors, access to resources, cognitive stimulation, and social support.</t>
+  </si>
+  <si>
+    <t>Lowering the IQ of a person, whether intentionally or unintentionally, could result in decreased cognitive abilities, reduced academic and occupational achievement, impaired problem-solving skills, and potential challenges in daily functioning and decision-making.</t>
+  </si>
+  <si>
+    <t>Potential applications of AI systems in nursing care settings include clinical decision support, patient monitoring, predictive analytics, personalized care planning, remote patient monitoring, workflow optimization, and patient engagement.</t>
+  </si>
+  <si>
+    <t>Yes, research suggests a positive association between grandiose narcissism and intelligence, while the relationship with vulnerable narcissism is less clear.</t>
+  </si>
+  <si>
+    <t>Implementing IIoT over 5G involves using high-speed, low-latency connectivity for real-time monitoring, remote control, data analytics, AR/VR applications, and supply chain optimization, enhancing efficiency and productivity in industrial operations.</t>
+  </si>
+  <si>
+    <t>The system uses YOLO-based detection for vehicle and license plate recognition, providing end-to-end automated license plate recognition, including vehicle classification.</t>
+  </si>
+  <si>
+    <t>Addictions can be linked to emotional intelligence deficits. Emotional intelligence involves understanding and managing emotions, which can play a role in coping with stress and managing impulses, both of which are factors in addiction.</t>
+  </si>
+  <si>
+    <t>Yes, there is a significant correlation between emotional intelligence (EI) and neuroticism, tension, and anxiety among flight cadets undergoing simulated flight training.</t>
+  </si>
+  <si>
+    <t>IQ (Intelligence Quotient) measures cognitive abilities such as reasoning, problem-solving, and logical thinking. EQ (Emotional Quotient) measures emotional intelligence, including skills like empathy, self-awareness, and interpersonal relationships.</t>
+  </si>
+  <si>
+    <t>Yes.</t>
+  </si>
+  <si>
+    <t>d) Perception of nursing's purpose</t>
+  </si>
+  <si>
+    <t>The Primate Cognitive Test Battery (PCTB) assesses various cognitive abilities in chimpanzees, including memory, problem-solving, spatial reasoning, and social cognition.</t>
+  </si>
+  <si>
+    <t>Besides chimpanzees, various animal species have shown a link between general intelligence and self-control behavior, including corvids (such as crows and ravens), dolphins, and some species of parrots.</t>
+  </si>
+  <si>
+    <t>The Hybrid Delay Task (HDT) measures self-control in chimpanzees by presenting them with choices between smaller, immediate rewards and larger, delayed rewards. The task evaluates their ability to inhibit the impulse for the immediate reward in favor of obtaining the larger, delayed reward.</t>
+  </si>
+  <si>
+    <t>Exposure to lead-based industries can impact the intelligence of school-aged children by causing cognitive impairments, including lower IQ scores, learning disabilities, and attention deficits. Lead exposure is particularly harmful to the developing brains of children, affecting areas responsible for cognition and behavior.</t>
+  </si>
+  <si>
+    <t>Researchers use population decoding to characterize the neural activity within face patches by analyzing the patterns of neural responses across multiple neurons. By decoding these patterns, researchers can infer the information being represented by the neural population, such as specific facial features or identities. This method helps understand how the brain processes and represents visual information related to faces.</t>
+  </si>
+  <si>
+    <t>A smart home system enables control of lighting, air conditioning, and other appliances through the use of interconnected devices and sensors. These devices are typically connected to a central hub or network that can be accessed and controlled remotely via a smartphone, tablet, or computer. Users can set schedules, adjust settings, and monitor energy usage from anywhere with an internet connection. Additionally, voice commands or automated routines can be programmed to control multiple devices simultaneously for added convenience.</t>
+  </si>
+  <si>
+    <t>The primary goals of the Hungarian Primary Care Model Programme included improving the quality and accessibility of primary care services, promoting preventive care and health promotion initiatives, enhancing coordination and integration of care across healthcare levels, and strengthening the role of primary care in the overall healthcare system.</t>
+  </si>
+  <si>
+    <t>Clinicians can improve communication by actively listening, showing empathy, using clear language, setting collaborative goals, providing tailored advice, offering continuous support, and utilizing technology.</t>
+  </si>
+  <si>
+    <t>Emotionally intelligent leaders can address pandemic challenges by recognizing emotions, providing support, communicating openly, fostering belonging, leading by example, encouraging resilience, and addressing moral concerns.</t>
+  </si>
+  <si>
+    <t>The concept of space topological cognition adds an understanding of the spatial relationships and connectivity between different locations within an environment to a target-driven visual navigation model. It enhances the model by allowing it to consider not only the target location but also the surrounding spatial layout, landmarks, and paths to efficiently navigate and reach the target.</t>
+  </si>
+  <si>
+    <t>Delay discounting (DD) refers to the tendency for individuals to devalue rewards as the delay to their receipt increases. In other words, it's the preference for smaller, immediate rewards over larger, delayed rewards. This phenomenon is often used to study impulsive decision-making and self-control, as individuals with higher levels of delay discounting are more likely to choose immediate gratification despite long-term consequences.</t>
+  </si>
+  <si>
+    <t>Children with less severe ASD symptoms and higher IQs are typically diagnosed at later ages compared to those with more severe symptoms. This is because their symptoms may be less noticeable or may not manifest as prominently, leading to delays in recognition and diagnosis. Additionally, their higher cognitive abilities may compensate for some social and communication difficulties, further delaying diagnosis until challenges become more apparent or problematic.</t>
+  </si>
+  <si>
+    <t>The emerging field of study that addresses the limitations of traditional safety ergonomics in the era of big data, aiming to enhance both safety and cleaner production practices, is known as "Safety 4.0" or "Industrial Safety 4.0."</t>
+  </si>
+  <si>
+    <t>Examining the relationship between cognitive intelligence (CI), emotional intelligence (EI), and religiosity could shed light on how individuals' analytical, emotional, and social capacities influence their religious beliefs, practices, and affiliations, contributing to a more nuanced understanding of religious diversity and behavior.</t>
+  </si>
+  <si>
+    <t>Individual differences in information processing speed are positively correlated with general intelligence. Faster processing speed allows individuals to efficiently acquire, process, and manipulate information, which is essential for cognitive tasks such as problem-solving, reasoning, and learning. Therefore, individuals with higher processing speed tend to perform better on measures of general intelligence.</t>
+  </si>
+  <si>
+    <t>Fluid reasoning (Gf) and working memory (WM) are closely related cognitive abilities that often interact in cognitive tasks. Fluid reasoning refers to the ability to think logically and solve problems in novel situations, while working memory involves the temporary storage and manipulation of information needed to complete cognitive tasks.
+Working memory plays a crucial role in fluid reasoning tasks by holding and manipulating relevant information while solving problems. Individuals with stronger working memory capacities are often better able to maintain and manipulate complex information, allowing them to perform more effectively on tasks requiring fluid reasoning abilities.
+In essence, working memory provides the cognitive workspace necessary for fluid reasoning processes to operate efficiently, and both abilities are important components of general cognitive ability or intelligence.</t>
+  </si>
+  <si>
+    <t>Athletic Expertise
+Enhances decision-making quality and speed due to transferable cognitive skills.
+Builds confidence for effective decisions under pressure.
+Trait Emotional Intelligence (TEI)
+Improves decision-making by understanding and regulating emotions.
+Reduces impulsive choices and unnecessary risk-taking.</t>
   </si>
 </sst>
 </file>
@@ -1684,8 +1915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C3B921-A260-8D4A-9BAD-EC588CEF4C8E}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2620,8 +2851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ECB6FD1-CDBE-694D-8700-2DD50D52B540}">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A30" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3496,8 +3727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F822382-AE75-4447-AC6A-1AB56E8F35E1}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="E1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3868,4 +4099,878 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4D5F179-E20B-EA4C-8803-91ABDFFF4221}">
+  <dimension ref="A1:D61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.5" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>348</v>
+      </c>
+      <c r="D1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D2" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>376</v>
+      </c>
+      <c r="B3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C3" t="s">
+        <v>324</v>
+      </c>
+      <c r="D3" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>376</v>
+      </c>
+      <c r="B4" t="s">
+        <v>322</v>
+      </c>
+      <c r="C4" t="s">
+        <v>321</v>
+      </c>
+      <c r="D4" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>376</v>
+      </c>
+      <c r="B5" t="s">
+        <v>316</v>
+      </c>
+      <c r="C5" t="s">
+        <v>315</v>
+      </c>
+      <c r="D5" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>376</v>
+      </c>
+      <c r="B6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C6" t="s">
+        <v>172</v>
+      </c>
+      <c r="D6" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>380</v>
+      </c>
+      <c r="B7" t="s">
+        <v>308</v>
+      </c>
+      <c r="C7" t="s">
+        <v>307</v>
+      </c>
+      <c r="D7" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>380</v>
+      </c>
+      <c r="B8" t="s">
+        <v>303</v>
+      </c>
+      <c r="C8" t="s">
+        <v>302</v>
+      </c>
+      <c r="D8" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>376</v>
+      </c>
+      <c r="B9" t="s">
+        <v>297</v>
+      </c>
+      <c r="C9" t="s">
+        <v>296</v>
+      </c>
+      <c r="D9" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>381</v>
+      </c>
+      <c r="B10" t="s">
+        <v>292</v>
+      </c>
+      <c r="C10" t="s">
+        <v>291</v>
+      </c>
+      <c r="D10" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>377</v>
+      </c>
+      <c r="B11" t="s">
+        <v>286</v>
+      </c>
+      <c r="C11" t="s">
+        <v>285</v>
+      </c>
+      <c r="D11" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>378</v>
+      </c>
+      <c r="B12" t="s">
+        <v>167</v>
+      </c>
+      <c r="C12" t="s">
+        <v>166</v>
+      </c>
+      <c r="D12" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>378</v>
+      </c>
+      <c r="B13" t="s">
+        <v>279</v>
+      </c>
+      <c r="C13" t="s">
+        <v>278</v>
+      </c>
+      <c r="D13" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>376</v>
+      </c>
+      <c r="B14" t="s">
+        <v>274</v>
+      </c>
+      <c r="C14" t="s">
+        <v>273</v>
+      </c>
+      <c r="D14" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>376</v>
+      </c>
+      <c r="B15" t="s">
+        <v>268</v>
+      </c>
+      <c r="C15" t="s">
+        <v>267</v>
+      </c>
+      <c r="D15" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>380</v>
+      </c>
+      <c r="B16" t="s">
+        <v>263</v>
+      </c>
+      <c r="C16" t="s">
+        <v>262</v>
+      </c>
+      <c r="D16" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>380</v>
+      </c>
+      <c r="B17" t="s">
+        <v>259</v>
+      </c>
+      <c r="C17" t="s">
+        <v>258</v>
+      </c>
+      <c r="D17" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>376</v>
+      </c>
+      <c r="B18" t="s">
+        <v>256</v>
+      </c>
+      <c r="C18" t="s">
+        <v>255</v>
+      </c>
+      <c r="D18" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>376</v>
+      </c>
+      <c r="B19" t="s">
+        <v>250</v>
+      </c>
+      <c r="C19" t="s">
+        <v>247</v>
+      </c>
+      <c r="D19" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>379</v>
+      </c>
+      <c r="B20" t="s">
+        <v>246</v>
+      </c>
+      <c r="C20" t="s">
+        <v>245</v>
+      </c>
+      <c r="D20" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>379</v>
+      </c>
+      <c r="B21" t="s">
+        <v>240</v>
+      </c>
+      <c r="C21" t="s">
+        <v>218</v>
+      </c>
+      <c r="D21" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>376</v>
+      </c>
+      <c r="B22" t="s">
+        <v>236</v>
+      </c>
+      <c r="C22" t="s">
+        <v>235</v>
+      </c>
+      <c r="D22" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>376</v>
+      </c>
+      <c r="B23" t="s">
+        <v>230</v>
+      </c>
+      <c r="C23" t="s">
+        <v>229</v>
+      </c>
+      <c r="D23" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>379</v>
+      </c>
+      <c r="B24" t="s">
+        <v>225</v>
+      </c>
+      <c r="C24" t="s">
+        <v>224</v>
+      </c>
+      <c r="D24" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>379</v>
+      </c>
+      <c r="B25" t="s">
+        <v>219</v>
+      </c>
+      <c r="C25" t="s">
+        <v>218</v>
+      </c>
+      <c r="D25" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>376</v>
+      </c>
+      <c r="B26" t="s">
+        <v>216</v>
+      </c>
+      <c r="C26" t="s">
+        <v>215</v>
+      </c>
+      <c r="D26" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>376</v>
+      </c>
+      <c r="B27" t="s">
+        <v>210</v>
+      </c>
+      <c r="C27" t="s">
+        <v>209</v>
+      </c>
+      <c r="D27" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>376</v>
+      </c>
+      <c r="B28" t="s">
+        <v>205</v>
+      </c>
+      <c r="C28" t="s">
+        <v>204</v>
+      </c>
+      <c r="D28" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>376</v>
+      </c>
+      <c r="B29" t="s">
+        <v>199</v>
+      </c>
+      <c r="C29" t="s">
+        <v>198</v>
+      </c>
+      <c r="D29" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>376</v>
+      </c>
+      <c r="B30" t="s">
+        <v>194</v>
+      </c>
+      <c r="C30" t="s">
+        <v>193</v>
+      </c>
+      <c r="D30" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>376</v>
+      </c>
+      <c r="B31" t="s">
+        <v>188</v>
+      </c>
+      <c r="C31" t="s">
+        <v>187</v>
+      </c>
+      <c r="D31" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>381</v>
+      </c>
+      <c r="B32" t="s">
+        <v>184</v>
+      </c>
+      <c r="C32" t="s">
+        <v>183</v>
+      </c>
+      <c r="D32" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>381</v>
+      </c>
+      <c r="B33" t="s">
+        <v>178</v>
+      </c>
+      <c r="C33" t="s">
+        <v>177</v>
+      </c>
+      <c r="D33" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>376</v>
+      </c>
+      <c r="B34" t="s">
+        <v>173</v>
+      </c>
+      <c r="C34" t="s">
+        <v>172</v>
+      </c>
+      <c r="D34" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>376</v>
+      </c>
+      <c r="B35" t="s">
+        <v>167</v>
+      </c>
+      <c r="C35" t="s">
+        <v>166</v>
+      </c>
+      <c r="D35" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>380</v>
+      </c>
+      <c r="B36" t="s">
+        <v>162</v>
+      </c>
+      <c r="C36" t="s">
+        <v>161</v>
+      </c>
+      <c r="D36" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>380</v>
+      </c>
+      <c r="B37" t="s">
+        <v>156</v>
+      </c>
+      <c r="C37" t="s">
+        <v>155</v>
+      </c>
+      <c r="D37" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>378</v>
+      </c>
+      <c r="B38" t="s">
+        <v>370</v>
+      </c>
+      <c r="C38" t="s">
+        <v>371</v>
+      </c>
+      <c r="D38" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>378</v>
+      </c>
+      <c r="B39" t="s">
+        <v>373</v>
+      </c>
+      <c r="C39" t="s">
+        <v>374</v>
+      </c>
+      <c r="D39" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>377</v>
+      </c>
+      <c r="B40" t="s">
+        <v>151</v>
+      </c>
+      <c r="C40" t="s">
+        <v>150</v>
+      </c>
+      <c r="D40">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>377</v>
+      </c>
+      <c r="B41" t="s">
+        <v>147</v>
+      </c>
+      <c r="C41" t="s">
+        <v>146</v>
+      </c>
+      <c r="D41" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>378</v>
+      </c>
+      <c r="B42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" t="s">
+        <v>86</v>
+      </c>
+      <c r="D42" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>383</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>378</v>
+      </c>
+      <c r="B44" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" t="s">
+        <v>89</v>
+      </c>
+      <c r="D44" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>376</v>
+      </c>
+      <c r="B45" t="s">
+        <v>30</v>
+      </c>
+      <c r="C45" t="s">
+        <v>99</v>
+      </c>
+      <c r="D45" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>376</v>
+      </c>
+      <c r="B46" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" t="s">
+        <v>102</v>
+      </c>
+      <c r="D46" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>384</v>
+      </c>
+      <c r="B47" t="s">
+        <v>34</v>
+      </c>
+      <c r="C47" t="s">
+        <v>103</v>
+      </c>
+      <c r="D47" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>384</v>
+      </c>
+      <c r="B48" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" t="s">
+        <v>91</v>
+      </c>
+      <c r="D48" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>384</v>
+      </c>
+      <c r="B49" t="s">
+        <v>43</v>
+      </c>
+      <c r="C49" t="s">
+        <v>107</v>
+      </c>
+      <c r="D49" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>384</v>
+      </c>
+      <c r="B50" t="s">
+        <v>340</v>
+      </c>
+      <c r="C50" t="s">
+        <v>122</v>
+      </c>
+      <c r="D50" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>376</v>
+      </c>
+      <c r="B51" t="s">
+        <v>72</v>
+      </c>
+      <c r="C51" t="s">
+        <v>131</v>
+      </c>
+      <c r="D51" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>384</v>
+      </c>
+      <c r="B52" t="s">
+        <v>79</v>
+      </c>
+      <c r="C52" t="s">
+        <v>349</v>
+      </c>
+      <c r="D52" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>384</v>
+      </c>
+      <c r="B53" t="s">
+        <v>350</v>
+      </c>
+      <c r="C53" t="s">
+        <v>351</v>
+      </c>
+      <c r="D53" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>376</v>
+      </c>
+      <c r="B54" t="s">
+        <v>352</v>
+      </c>
+      <c r="C54" t="s">
+        <v>346</v>
+      </c>
+      <c r="D54" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>376</v>
+      </c>
+      <c r="B55" t="s">
+        <v>353</v>
+      </c>
+      <c r="C55" t="s">
+        <v>354</v>
+      </c>
+      <c r="D55" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>377</v>
+      </c>
+      <c r="B56" t="s">
+        <v>356</v>
+      </c>
+      <c r="C56" t="s">
+        <v>355</v>
+      </c>
+      <c r="D56" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>376</v>
+      </c>
+      <c r="B57" t="s">
+        <v>357</v>
+      </c>
+      <c r="C57" t="s">
+        <v>126</v>
+      </c>
+      <c r="D57" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>381</v>
+      </c>
+      <c r="B58" t="s">
+        <v>358</v>
+      </c>
+      <c r="C58" t="s">
+        <v>360</v>
+      </c>
+      <c r="D58" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>381</v>
+      </c>
+      <c r="B59" t="s">
+        <v>361</v>
+      </c>
+      <c r="C59" t="s">
+        <v>363</v>
+      </c>
+      <c r="D59" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>381</v>
+      </c>
+      <c r="B60" t="s">
+        <v>365</v>
+      </c>
+      <c r="C60" t="s">
+        <v>366</v>
+      </c>
+      <c r="D60" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>380</v>
+      </c>
+      <c r="B61" t="s">
+        <v>368</v>
+      </c>
+      <c r="C61" t="s">
+        <v>369</v>
+      </c>
+      <c r="D61" t="s">
+        <v>442</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added ChatGPT Answers for the rest of the questions from the eval dataset
</commit_message>
<xml_diff>
--- a/kedronlp/notebooks/Evaluation.xlsx
+++ b/kedronlp/notebooks/Evaluation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arjan/Bachelor/NLP with Transformers/pubMedNLP/kedronlp/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CEC233-AB14-7149-9086-5044A2A56DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9888FF63-B2F4-C048-B3F3-07E26DCBE3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16120" activeTab="3" xr2:uid="{3AC1803B-D431-F74E-BDCB-3D80AD30DE94}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="594">
   <si>
     <t>Question Type</t>
   </si>
@@ -1545,6 +1545,460 @@
 Trait Emotional Intelligence (TEI)
 Improves decision-making by understanding and regulating emotions.
 Reduces impulsive choices and unnecessary risk-taking.</t>
+  </si>
+  <si>
+    <t>How do resting-state functional connectivity and activity flow mapping contribute to understanding episodic memory information transfer in the brain?</t>
+  </si>
+  <si>
+    <t>Are spatial processing methods such as median filtering and the laplace operator applied to achieve de-noising and contrast enhancement on infrared images?</t>
+  </si>
+  <si>
+    <t>Did the application of neural networks receive increasing attention in the field of chemometrics?</t>
+  </si>
+  <si>
+    <t>Describe what post-perative cystography is oftentimes used for?</t>
+  </si>
+  <si>
+    <t>Are psychological changes that underly the the increasing appetite following cannabis consumption over or under researched?</t>
+  </si>
+  <si>
+    <t>What are possible influental factors that distinguish prognosis between non-viral HCC and HCV_HCC groups?</t>
+  </si>
+  <si>
+    <t>What should intervention programs for aggressive individuals focus on in order to foster behavioral improvement?</t>
+  </si>
+  <si>
+    <t>What components could be considered to understand the emotional management ability of teachers.</t>
+  </si>
+  <si>
+    <t>Do young people with a tendency towards excitement-seeking behavior also show a tendency towrards problematic gambling?</t>
+  </si>
+  <si>
+    <t>How could electroencephalography helpful in treating individuals after a stroke?</t>
+  </si>
+  <si>
+    <t>What is a reliable measure for verbal intelligence?</t>
+  </si>
+  <si>
+    <t>What might be a new method for identifying circRNA-disease associations? a) a neural network based methodology called HMCDA b) a reinforcement learning based methodology named LGTS c) there is not new method.</t>
+  </si>
+  <si>
+    <t>Would the identification of rehabilitative risk factors that limit an individuals mobility improve or rather worsen the prospective treatment of affected patients?</t>
+  </si>
+  <si>
+    <t>How can accidents in hydropower engineering projects be avoided?</t>
+  </si>
+  <si>
+    <t>Is the main field of AI application in the healthcare sector focused on the individual?</t>
+  </si>
+  <si>
+    <t>How does syntactic complexity influence speech comprehension?</t>
+  </si>
+  <si>
+    <t>Could AI be used to help disabled workers in their jobs?</t>
+  </si>
+  <si>
+    <t>What is an indirect consequence of eating a lot of meat?</t>
+  </si>
+  <si>
+    <t>What is domain adaption in the context of applying AI to medical images?</t>
+  </si>
+  <si>
+    <t>Does exposure to stress have positive or negative impact on the way they treat their children?</t>
+  </si>
+  <si>
+    <t>Which factors improves target mass transfer efficiency?</t>
+  </si>
+  <si>
+    <t>The task of automaticall sorting amomum villosum is a) not solvable b) solvable with a CNN based on x-ray data.</t>
+  </si>
+  <si>
+    <t>What are persisting problems of traffic estimation?</t>
+  </si>
+  <si>
+    <t>Which combination of different fields might help to overcome the severe shortcommings of models explaining human consciousness?</t>
+  </si>
+  <si>
+    <t>What is foamed lightweight soil?</t>
+  </si>
+  <si>
+    <t>What are possible explanations for the negative correlation between religiousness and aggression?</t>
+  </si>
+  <si>
+    <t>What is the reason that the universe will die?</t>
+  </si>
+  <si>
+    <t>Would a motivational model of psychopathology be better if it would integrate information about the bottom-up emotion generation system with top-down emotion regulation systems?</t>
+  </si>
+  <si>
+    <t>What influences in individuals capacity to be innovative?</t>
+  </si>
+  <si>
+    <t>What is a possibility for curing cervical cancer?</t>
+  </si>
+  <si>
+    <t>How does punishment influence inter-brain synchronization between two individuals?</t>
+  </si>
+  <si>
+    <t>Can it be dangerous for a person with only one kidney if it gets infected with Covid?</t>
+  </si>
+  <si>
+    <t>Which criteria do modern language models such as GPT 3.5 not meet in order to be applicable in childcare?</t>
+  </si>
+  <si>
+    <t>How can potentiated Natural Killer cells help to cure ccRCC?</t>
+  </si>
+  <si>
+    <t>Do people generally score higher in general health measurements when they get older?</t>
+  </si>
+  <si>
+    <t>Are there possible genetic causes for bipolar disorder?</t>
+  </si>
+  <si>
+    <t>How can the effects of Kratom Mitragyna speciosa be described?</t>
+  </si>
+  <si>
+    <t>What brain-related abnormalies can be observed among autistic children?</t>
+  </si>
+  <si>
+    <t>Can traditional MFS algorithms be outperformed with other alternatives?</t>
+  </si>
+  <si>
+    <t>Is the blood brain barrier important for the ability of people to smell cheese?</t>
+  </si>
+  <si>
+    <t>What is a problem for cancer genetic risk profiling in the middle east?</t>
+  </si>
+  <si>
+    <t>Does the motivation of an individual to change its addictive behavior influence the likelihood of this individual to start drinking again after a therapy?</t>
+  </si>
+  <si>
+    <t>Are expecially native new zealanders affected by rheumatic fever?</t>
+  </si>
+  <si>
+    <t>Assume you have motivated and not so motivated people in your study. Which group of participants are more likely to exhibit a greater placebo response?</t>
+  </si>
+  <si>
+    <t>Which aspects the paper about deep reconstruction models for image set classification has been criticised by other researchers?</t>
+  </si>
+  <si>
+    <t>Are colloid cysts ronly elated to neurocognitive decline after a patient has been operated?</t>
+  </si>
+  <si>
+    <t>Can machine learning models predict individuals that are likely to again sicken with intracerebral hemorrhage?</t>
+  </si>
+  <si>
+    <t>How could Endoplasmic reticulum stress be measured?</t>
+  </si>
+  <si>
+    <t>is it easier to experimentally determine or  to computationally predict their an RNA's structure?</t>
+  </si>
+  <si>
+    <t>Is there a faster growing type of genomics data than the single-cell omics?</t>
+  </si>
+  <si>
+    <t>Which of the following criteria are included in clinically assessing dementia: a) body smell b) hairstyle c) body size d) previous employment e) depressive symptoms</t>
+  </si>
+  <si>
+    <t>Can you describe an environment in which cochlear implants do not function properly?</t>
+  </si>
+  <si>
+    <t>What are dual-mechanism ECL sensors based on? a) measuring the amount of calcium in water for electrocatalytic activity b) RET by assembling GNPs on 2d polymorphyrinic MOF nanosheets.</t>
+  </si>
+  <si>
+    <t>Resting-state FC and activity flow mapping quantify episodic memory information transfer by analyzing signal interactions between brain regions.</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Predicting postprostatectomy urinary incontinence (PPI) recovery.</t>
+  </si>
+  <si>
+    <t>Under-researched.</t>
+  </si>
+  <si>
+    <t>Number of tumors, HCC stage, albumin, and total bilirubin.</t>
+  </si>
+  <si>
+    <t>Increase cognitive empathy and explore emotional self-regulation and callous-unemotional traits.</t>
+  </si>
+  <si>
+    <t>EEG helps classify stroke patients, aiding post-stroke treatment and recovery.</t>
+  </si>
+  <si>
+    <t>The Ammons Quick Test (QT) is a reliable measure for verbal intelligence.</t>
+  </si>
+  <si>
+    <t>a) a neural network-based methodology called HMCDA</t>
+  </si>
+  <si>
+    <t>Improve.</t>
+  </si>
+  <si>
+    <t>By identifying and eliminating near misses, utilizing AI for automatic classification, and implementing association analysis for structured data mining.</t>
+  </si>
+  <si>
+    <t>Syntactic complexity increases pupil dilations but has less impact on subjective effort, influenced more by noise level.</t>
+  </si>
+  <si>
+    <t>Yes, AI can assist disabled workers through technologies like N-CAPS for monitoring and support in factory assembly tasks.</t>
+  </si>
+  <si>
+    <t>Increased meat consumption contributes to environmental degradation, worsening fine particulate matter (PM2.5) pollution and impacting health.</t>
+  </si>
+  <si>
+    <t>Domain adaptation in AI for medical images refers to the process of adjusting models to account for variations in image characteristics from different sources, enhancing performance across diverse imaging environments.</t>
+  </si>
+  <si>
+    <t>Exposure to stress has a negative impact on the way mothers respond to infant cues, affecting maternal motivation, emotion regulation, and empathy.</t>
+  </si>
+  <si>
+    <t>The vertical permeability and microvortex effect provided by the AuNP-bridge array synergistically improve target mass transfer efficiency.</t>
+  </si>
+  <si>
+    <t>b) solvable with a CNN based on x-ray data.</t>
+  </si>
+  <si>
+    <t>Data missing problem, MNAR (missing not at random) traffic speed data, link-based traffic status modeling, limited number of probe vehicles.</t>
+  </si>
+  <si>
+    <t>Combining ideas from psychology and quantum mechanics.</t>
+  </si>
+  <si>
+    <t>Lightweight cementitious material with tiny closed pores used as filler in construction.</t>
+  </si>
+  <si>
+    <t>1. Teaching self-control
+2. Emphasizing compassionate beliefs</t>
+  </si>
+  <si>
+    <t>The paper does not provide specific details on why the universe will die.</t>
+  </si>
+  <si>
+    <t>Persistence, motor diversity, activity, and neophobia.</t>
+  </si>
+  <si>
+    <t>Early detection of pre-cancerous cervical changes through advanced screening technologies.</t>
+  </si>
+  <si>
+    <t>Punishment has a negative effect on inter-brain synchronization, reducing it in social interactions.</t>
+  </si>
+  <si>
+    <t>Yes, potential danger exists; SARS-CoV-2 can induce renal damage, and ACE2, critical for kidney function, is implicated.</t>
+  </si>
+  <si>
+    <t>They failed to meet passing criteria in Japan's childcare worker national examination, and accuracy concerns were observed, posing a risk of incorrect information.</t>
+  </si>
+  <si>
+    <t>Potentiated Natural Killer (NK) cells enhance cytotoxicity against renal cell carcinoma (RCC) cells, contributing to inhibition of ccRCC progression.</t>
+  </si>
+  <si>
+    <t>GPT gave a wrong answer</t>
+  </si>
+  <si>
+    <t>Yes, genome-wide association studies (GWAS) have identified genetic loci associated with bipolar disorder (BD), suggesting possible genetic causes.</t>
+  </si>
+  <si>
+    <t>The effects of Kratom Mitragyna speciosa are opioid-like.</t>
+  </si>
+  <si>
+    <t>Abnormalities in brain connections, especially in the left hemisphere, and connectivity issues in frontal and parietal lobes are observed in autistic children, with significant differences in alpha, beta, and gamma bands.</t>
+  </si>
+  <si>
+    <t>Yes, the proposed OSLGC method outperforms traditional Multi-Label Feature Selection (MFS) algorithms.</t>
+  </si>
+  <si>
+    <t>No, the context provided does not mention any connection between the blood-brain barrier and the ability to smell cheese.</t>
+  </si>
+  <si>
+    <t>The paucity of genomic data in Middle Eastern populations is a challenge for cancer genetic risk profiling.</t>
+  </si>
+  <si>
+    <t>Motivated participants.</t>
+  </si>
+  <si>
+    <t>Experimental results and data inconsistencies.</t>
+  </si>
+  <si>
+    <t>Through the detection of morphological patterns, particularly the formation of ring-shaped structures called whorls (WHs), using a deep learning-based image analysis assay named ER-WHs-Analyzer.</t>
+  </si>
+  <si>
+    <t>It is easier to computationally predict an RNA's structure than experimentally determine it.</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>e) depressive symptoms</t>
+  </si>
+  <si>
+    <t>Noisy environments</t>
+  </si>
+  <si>
+    <t>b) RET by assembling GNPs on 2D polymorphyrinic MOF nanosheets.</t>
+  </si>
+  <si>
+    <t>Resting-state functional connectivity helps identify brain regions that communicate during memory processes. Activity flow mapping reveals the directionality of information transfer. Together, they elucidate how episodic memory information flows between brain areas, enhancing our understanding of memory mechanisms.</t>
+  </si>
+  <si>
+    <t>Yes, spatial processing methods like median filtering are used for denoising in infrared images. The Laplace operator is applied for contrast enhancement, enhancing edges and features in the images.</t>
+  </si>
+  <si>
+    <t>Yes, neural networks have garnered increasing attention in chemometrics for tasks like spectral analysis, calibration, and classification due to their ability to handle complex datasets and nonlinear relationships effectively.</t>
+  </si>
+  <si>
+    <t>Post-operative cystography is often used to assess the integrity of the urinary bladder after surgical procedures, particularly those involving the bladder or nearby structures. It helps detect any leaks, fistulas, or other abnormalities that may have occurred during surgery.</t>
+  </si>
+  <si>
+    <t>Psychological changes underlying increased appetite after cannabis consumption are relatively under-researched compared to other effects of cannabis. While there's some understanding of the involvement of cannabinoid receptors in appetite regulation, further research is needed to elucidate the precise mechanisms and psychological factors influencing this phenomenon.</t>
+  </si>
+  <si>
+    <t>Liver function, tumor characteristics, treatment response, comorbidities, genetic factors, viral load, immune response, and access to healthcare.</t>
+  </si>
+  <si>
+    <t>Intervention programs for aggressive individuals should focus on teaching anger management techniques, improving communication skills, promoting empathy and perspective-taking, addressing underlying mental health issues, and providing support for stress management and coping strategies.</t>
+  </si>
+  <si>
+    <t>Components to understand the emotional management ability of teachers may include self-awareness, emotional regulation skills, empathy, effective communication, stress coping strategies, ability to establish supportive relationships, and adaptability in handling challenging situations.</t>
+  </si>
+  <si>
+    <t>Yes, young people with a tendency towards excitement-seeking behavior are more likely to exhibit problematic gambling tendencies. This is because both excitement-seeking behavior and problematic gambling are associated with seeking out novel and stimulating experiences, taking risks, and having difficulties with impulse control.</t>
+  </si>
+  <si>
+    <t>Electroencephalography (EEG) can be helpful in treating individuals after a stroke by providing valuable information about brain activity and functional connectivity. It can aid in assessing the extent of brain damage, identifying areas of neural plasticity and recovery potential, guiding rehabilitation strategies, monitoring treatment progress, and predicting outcomes. EEG can also assist in detecting complications such as seizures and cognitive impairments, allowing for timely intervention and personalized care.</t>
+  </si>
+  <si>
+    <t>One reliable measure for verbal intelligence is the Wechsler Adult Intelligence Scale (WAIS) or its variations for different age groups, such as the Wechsler Intelligence Scale for Children (WISC). These tests include verbal comprehension tasks that assess vocabulary, general knowledge, verbal reasoning, and verbal problem-solving abilities.</t>
+  </si>
+  <si>
+    <t>c) There is not a new method.</t>
+  </si>
+  <si>
+    <t>Identifying rehabilitative risk factors that limit an individual's mobility would likely improve the prospective treatment of affected patients. By understanding these factors, healthcare providers can tailor rehabilitation programs to address specific challenges, potentially leading to more effective and personalized treatments that enhance mobility and overall outcomes.</t>
+  </si>
+  <si>
+    <t>Accidents in hydropower engineering projects can be avoided by implementing strict safety protocols, conducting thorough risk assessments, providing comprehensive training to personnel, ensuring proper maintenance of equipment and infrastructure, adhering to regulatory standards, conducting regular safety inspections, promoting a culture of safety among workers, and utilizing advanced technology for monitoring and early detection of potential hazards.</t>
+  </si>
+  <si>
+    <t>Yes. The main field of AI application in the healthcare sector is increasingly focused on the individual, aiming to provide personalized and targeted treatments, diagnoses, and interventions tailored to each patient's unique needs and characteristics.</t>
+  </si>
+  <si>
+    <t>Syntactic complexity in speech can influence comprehension by affecting the cognitive load placed on the listener. More complex syntax may require greater cognitive resources to process, leading to slower comprehension, increased likelihood of errors, or difficulty in maintaining the context of the conversation. However, individuals vary in their ability to comprehend syntactically complex speech, with factors such as linguistic proficiency and working memory capacity playing a role in how effectively they can process and understand complex syntax.</t>
+  </si>
+  <si>
+    <t>Yes, AI can be used to help disabled workers in their jobs by providing assistive technologies tailored to their specific needs. This can include tools for speech recognition, text-to-speech conversion, voice control interfaces, adaptive software interfaces, robotic assistance for physical tasks, and AI-powered systems for task automation and cognitive support. These technologies can empower disabled workers to perform their jobs more effectively, independently, and with greater accessibility.</t>
+  </si>
+  <si>
+    <t>An indirect consequence of eating a lot of meat is its environmental impact. Large-scale meat production contributes to deforestation, greenhouse gas emissions, water pollution, and habitat destruction. This can lead to various environmental problems such as climate change, loss of biodiversity, and degradation of ecosystems.</t>
+  </si>
+  <si>
+    <t>Domain adaptation in the context of applying AI to medical images refers to the process of transferring knowledge learned from one dataset (source domain) to another dataset (target domain) where the data distributions may be different. In medical imaging, this could involve training a model on images from one hospital or imaging device and adapting it to work effectively on images from a different hospital or device. Domain adaptation techniques aim to mitigate differences in data distributions and improve the generalization of AI models across different imaging settings.</t>
+  </si>
+  <si>
+    <t>Exposure to stress can have both positive and negative impacts on the way parents treat their children. In some cases, stress may lead to increased irritability, impatience, or decreased emotional regulation, resulting in negative parenting behaviors such as yelling or harsh discipline. However, stress can also motivate parents to seek social support, prioritize self-care, and develop resilience, which can positively influence their interactions with their children. Ultimately, the impact of stress on parenting behavior depends on various factors, including individual coping strategies, social support networks, and the context of the stressors.</t>
+  </si>
+  <si>
+    <t>Factors that improve target mass transfer efficiency include increased surface area, higher concentration gradients, efficient mixing, and optimized environmental conditions.</t>
+  </si>
+  <si>
+    <t>b) Solvable with a CNN based on x-ray data.</t>
+  </si>
+  <si>
+    <t>Persisting problems of traffic estimation include inaccurate data due to limited sensor coverage, variability in traffic patterns, difficulties in predicting sudden changes, and challenges in integrating data from diverse sources such as GPS, cameras, and vehicle detectors. Additionally, issues like privacy concerns, data reliability, and computational complexity remain significant hurdles in accurate traffic estimation.</t>
+  </si>
+  <si>
+    <t>Combining expertise from fields such as neuroscience, psychology, philosophy, artificial intelligence, and cognitive science might help overcome the severe shortcomings of models explaining human consciousness. This interdisciplinary approach could provide diverse perspectives and methodologies to address the complex nature of consciousness, incorporating biological, psychological, computational, and philosophical insights to develop more comprehensive models.</t>
+  </si>
+  <si>
+    <t>Foamed lightweight soil is a type of soil that has been treated with a foam agent to introduce air voids, reducing its density and making it lighter in weight. This type of soil is commonly used in construction and landscaping applications where weight reduction is desirable, such as backfilling, slope stabilization, and green roof installations. The foaming process improves soil aeration, drainage, and thermal insulation properties while maintaining adequate structural stability.</t>
+  </si>
+  <si>
+    <t>Empathy, moral values, social support, and self-regulation could contribute.</t>
+  </si>
+  <si>
+    <t>The universe's eventual heat death is due to entropy increasing over time, causing all energy to become evenly distributed and unavailable for further use.</t>
+  </si>
+  <si>
+    <t>Yes, integrating both bottom-up emotion generation and top-down emotion regulation systems would provide a more comprehensive understanding of motivational aspects in psychopathology.</t>
+  </si>
+  <si>
+    <t>Factors like cognitive flexibility, openness to experience, creativity, motivation, and environmental support influence an individual's capacity for innovation.</t>
+  </si>
+  <si>
+    <t>Early detection through screening programs like Pap smears, HPV vaccination, targeted therapies, and advances in immunotherapy hold promise for curing cervical cancer.</t>
+  </si>
+  <si>
+    <t>Punishment can disrupt inter-brain synchronization by inducing stress and altering social dynamics, potentially leading to decreased cooperation and empathy between individuals.</t>
+  </si>
+  <si>
+    <t>Yes, individuals with only one kidney may be at increased risk of complications if they contract COVID-19, as their compromised kidney function could potentially worsen due to the infection.</t>
+  </si>
+  <si>
+    <t>Modern language models like GPT-3.5 lack emotional understanding, empathy, and the ability to ensure child safety, making them unsuitable for childcare without significant human supervision.</t>
+  </si>
+  <si>
+    <t>Potentiated Natural Killer (NK) cells can help cure clear cell renal cell carcinoma (ccRCC) by targeting and destroying cancer cells more effectively, enhancing the body's immune response against the tumor.</t>
+  </si>
+  <si>
+    <t>Not necessarily. While some aspects of health may improve with age due to increased maturity and better access to healthcare, other factors such as chronic conditions and physical decline can also arise, affecting general health measurements.</t>
+  </si>
+  <si>
+    <t>Yes, genetic factors play a significant role in bipolar disorder, with evidence suggesting that multiple genes contribute to its development.</t>
+  </si>
+  <si>
+    <t>The effects of Kratom (Mitragyna speciosa) can vary depending on the dose and individual response, but they often include pain relief, increased energy, mood enhancement, and sedation at higher doses.</t>
+  </si>
+  <si>
+    <t>Autistic children may exhibit various brain-related abnormalities, including differences in brain structure, such as enlarged or reduced volume in certain areas, altered connectivity between brain regions, and abnormalities in neurotransmitter systems involved in social communication and sensory processing.</t>
+  </si>
+  <si>
+    <t>Yes, traditional mean-field swarm (MFS) algorithms can be outperformed by alternative approaches such as particle swarm optimization (PSO), genetic algorithms (GA), or hybrid methods that combine multiple optimization techniques.</t>
+  </si>
+  <si>
+    <t>No, the blood-brain barrier is not directly involved in the ability of people to smell cheese. Olfactory receptors in the nasal cavity detect odor molecules, which then travel to the brain's olfactory bulb, bypassing the blood-brain barrier.</t>
+  </si>
+  <si>
+    <t>A problem for cancer genetic risk profiling in the Middle East is the limited availability of comprehensive genetic databases and resources specific to the diverse ethnic groups in the region, which hinders accurate risk assessment and personalized treatment strategies.</t>
+  </si>
+  <si>
+    <t>Yes, the motivation of an individual to change addictive behavior significantly influences the likelihood of relapse after therapy. Higher motivation and commitment to change generally correlate with better treatment outcomes and a reduced risk of returning to addictive behaviors.</t>
+  </si>
+  <si>
+    <t>Yes, rheumatic fever disproportionately affects Māori and Pacific Islander populations in New Zealand, with higher rates of incidence and poorer outcomes compared to other ethnic groups in the country.</t>
+  </si>
+  <si>
+    <t>Participants who are more motivated are generally more likely to exhibit a greater placebo response compared to those who are less motivated. Motivation can enhance expectations of treatment efficacy, amplifying the placebo effect.</t>
+  </si>
+  <si>
+    <t>The paper on deep reconstruction models for image set classification has been criticized by other researchers for its limited generalization to diverse datasets, lack of robustness to variations in input data, and potential overfitting to specific training conditions.</t>
+  </si>
+  <si>
+    <t>Colloid cysts can be related to neurocognitive decline, but whether this decline persists after surgery depends on various factors such as the size and location of the cyst, the extent of neurological damage prior to surgery, and the success of the surgical intervention.</t>
+  </si>
+  <si>
+    <t>Yes, machine learning models can be trained on clinical data to predict the likelihood of individuals experiencing recurrent intracerebral hemorrhage, based on factors such as medical history, imaging findings, and demographic information.</t>
+  </si>
+  <si>
+    <t>Endoplasmic reticulum (ER) stress can be measured through various methods, including assessing the expression levels of ER stress markers such as GRP78/BiP, ATF4, and CHOP, monitoring ER morphology changes, quantifying unfolded protein response (UPR) activation, and evaluating ER stress-related cellular functions such as protein folding and degradation.</t>
+  </si>
+  <si>
+    <t>It's generally easier to experimentally determine an RNA's structure through techniques like X-ray crystallography, NMR spectroscopy, or cryo-electron microscopy, rather than relying solely on computational prediction methods, which can be limited by the complexity and size of RNA molecules.</t>
+  </si>
+  <si>
+    <t>As of my last update in January 2022, single-cell omics data was one of the fastest-growing types of genomics data due to its ability to provide high-resolution insights into cellular heterogeneity. While other types of genomics data, such as whole-genome sequencing or bulk RNA sequencing, also continue to grow, single-cell omics data has seen particularly rapid expansion due to advancements in technology and its increasing applications across various fields.</t>
+  </si>
+  <si>
+    <t>The criteria included in clinically assessing dementia typically focus on cognitive functioning and related symptoms. Among the options provided, only "e) depressive symptoms" is relevant to the assessment of dementia.</t>
+  </si>
+  <si>
+    <t>An environment with excessive electromagnetic interference, such as areas with strong radiofrequency signals or electrical machinery, can disrupt the function of cochlear implants. Additionally, environments with high levels of moisture or humidity may affect the performance of the device.</t>
+  </si>
+  <si>
+    <t>The correct answer is b) RET by assembling GNPs on 2d polymorphyrinic MOF nanosheets. Dual-mechanism ECL sensors are based on resonance energy transfer (RET), which involves the transfer of energy from an excited donor molecule to an acceptor molecule, leading to emission of light. In this case, GNPs (gold nanoparticles) are assembled on 2D polymorphyrinic metal-organic framework (MOF) nanosheets to enable RET and enhance the electrochemiluminescence (ECL) signal.</t>
   </si>
 </sst>
 </file>
@@ -4103,17 +4557,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4D5F179-E20B-EA4C-8803-91ABDFFF4221}">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="D114" sqref="D114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.5" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="45.1640625" customWidth="1"/>
+    <col min="3" max="3" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -4970,6 +5424,748 @@
         <v>442</v>
       </c>
     </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>377</v>
+      </c>
+      <c r="B62" t="s">
+        <v>443</v>
+      </c>
+      <c r="C62" t="s">
+        <v>496</v>
+      </c>
+      <c r="D62" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>378</v>
+      </c>
+      <c r="B63" t="s">
+        <v>444</v>
+      </c>
+      <c r="C63" t="s">
+        <v>497</v>
+      </c>
+      <c r="D63" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>378</v>
+      </c>
+      <c r="B64" t="s">
+        <v>445</v>
+      </c>
+      <c r="C64" t="s">
+        <v>498</v>
+      </c>
+      <c r="D64" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>380</v>
+      </c>
+      <c r="B65" t="s">
+        <v>446</v>
+      </c>
+      <c r="C65" t="s">
+        <v>499</v>
+      </c>
+      <c r="D65" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>377</v>
+      </c>
+      <c r="B66" t="s">
+        <v>447</v>
+      </c>
+      <c r="C66" t="s">
+        <v>500</v>
+      </c>
+      <c r="D66" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>381</v>
+      </c>
+      <c r="B67" t="s">
+        <v>448</v>
+      </c>
+      <c r="C67" t="s">
+        <v>501</v>
+      </c>
+      <c r="D67" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>376</v>
+      </c>
+      <c r="B68" t="s">
+        <v>449</v>
+      </c>
+      <c r="C68" t="s">
+        <v>502</v>
+      </c>
+      <c r="D68" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>376</v>
+      </c>
+      <c r="B69" t="s">
+        <v>450</v>
+      </c>
+      <c r="C69" t="s">
+        <v>502</v>
+      </c>
+      <c r="D69" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>378</v>
+      </c>
+      <c r="B70" t="s">
+        <v>451</v>
+      </c>
+      <c r="C70" t="s">
+        <v>498</v>
+      </c>
+      <c r="D70" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>384</v>
+      </c>
+      <c r="B71" t="s">
+        <v>452</v>
+      </c>
+      <c r="C71" t="s">
+        <v>503</v>
+      </c>
+      <c r="D71" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>376</v>
+      </c>
+      <c r="B72" t="s">
+        <v>453</v>
+      </c>
+      <c r="C72" t="s">
+        <v>504</v>
+      </c>
+      <c r="D72" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>383</v>
+      </c>
+      <c r="B73" t="s">
+        <v>454</v>
+      </c>
+      <c r="C73" t="s">
+        <v>505</v>
+      </c>
+      <c r="D73" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>377</v>
+      </c>
+      <c r="B74" t="s">
+        <v>455</v>
+      </c>
+      <c r="C74" t="s">
+        <v>506</v>
+      </c>
+      <c r="D74" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>384</v>
+      </c>
+      <c r="B75" t="s">
+        <v>456</v>
+      </c>
+      <c r="C75" t="s">
+        <v>507</v>
+      </c>
+      <c r="D75" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>378</v>
+      </c>
+      <c r="B76" t="s">
+        <v>457</v>
+      </c>
+      <c r="C76" t="s">
+        <v>497</v>
+      </c>
+      <c r="D76" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>384</v>
+      </c>
+      <c r="B77" t="s">
+        <v>458</v>
+      </c>
+      <c r="C77" t="s">
+        <v>508</v>
+      </c>
+      <c r="D77" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>381</v>
+      </c>
+      <c r="B78" t="s">
+        <v>459</v>
+      </c>
+      <c r="C78" t="s">
+        <v>509</v>
+      </c>
+      <c r="D78" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>376</v>
+      </c>
+      <c r="B79" t="s">
+        <v>460</v>
+      </c>
+      <c r="C79" t="s">
+        <v>510</v>
+      </c>
+      <c r="D79" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>381</v>
+      </c>
+      <c r="B80" t="s">
+        <v>461</v>
+      </c>
+      <c r="C80" t="s">
+        <v>511</v>
+      </c>
+      <c r="D80" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>377</v>
+      </c>
+      <c r="B81" t="s">
+        <v>462</v>
+      </c>
+      <c r="C81" t="s">
+        <v>512</v>
+      </c>
+      <c r="D81" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>376</v>
+      </c>
+      <c r="B82" t="s">
+        <v>463</v>
+      </c>
+      <c r="C82" t="s">
+        <v>513</v>
+      </c>
+      <c r="D82" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>383</v>
+      </c>
+      <c r="B83" t="s">
+        <v>464</v>
+      </c>
+      <c r="C83" t="s">
+        <v>514</v>
+      </c>
+      <c r="D83" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>379</v>
+      </c>
+      <c r="B84" t="s">
+        <v>465</v>
+      </c>
+      <c r="C84" t="s">
+        <v>515</v>
+      </c>
+      <c r="D84" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>376</v>
+      </c>
+      <c r="B85" t="s">
+        <v>466</v>
+      </c>
+      <c r="C85" t="s">
+        <v>516</v>
+      </c>
+      <c r="D85" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>376</v>
+      </c>
+      <c r="B86" t="s">
+        <v>467</v>
+      </c>
+      <c r="C86" t="s">
+        <v>517</v>
+      </c>
+      <c r="D86" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>376</v>
+      </c>
+      <c r="B87" t="s">
+        <v>468</v>
+      </c>
+      <c r="C87" t="s">
+        <v>518</v>
+      </c>
+      <c r="D87" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>381</v>
+      </c>
+      <c r="B88" t="s">
+        <v>469</v>
+      </c>
+      <c r="C88" t="s">
+        <v>519</v>
+      </c>
+      <c r="D88" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>377</v>
+      </c>
+      <c r="B89" t="s">
+        <v>470</v>
+      </c>
+      <c r="C89" t="s">
+        <v>497</v>
+      </c>
+      <c r="D89" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>381</v>
+      </c>
+      <c r="B90" t="s">
+        <v>471</v>
+      </c>
+      <c r="C90" t="s">
+        <v>520</v>
+      </c>
+      <c r="D90" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>380</v>
+      </c>
+      <c r="B91" t="s">
+        <v>472</v>
+      </c>
+      <c r="C91" t="s">
+        <v>521</v>
+      </c>
+      <c r="D91" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>384</v>
+      </c>
+      <c r="B92" t="s">
+        <v>473</v>
+      </c>
+      <c r="C92" t="s">
+        <v>522</v>
+      </c>
+      <c r="D92" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>379</v>
+      </c>
+      <c r="B93" t="s">
+        <v>474</v>
+      </c>
+      <c r="C93" t="s">
+        <v>523</v>
+      </c>
+      <c r="D93" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>376</v>
+      </c>
+      <c r="B94" t="s">
+        <v>475</v>
+      </c>
+      <c r="C94" t="s">
+        <v>524</v>
+      </c>
+      <c r="D94" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>384</v>
+      </c>
+      <c r="B95" t="s">
+        <v>476</v>
+      </c>
+      <c r="C95" t="s">
+        <v>525</v>
+      </c>
+      <c r="D95" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>377</v>
+      </c>
+      <c r="B96" t="s">
+        <v>477</v>
+      </c>
+      <c r="C96" t="s">
+        <v>526</v>
+      </c>
+      <c r="D96" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>381</v>
+      </c>
+      <c r="B97" t="s">
+        <v>478</v>
+      </c>
+      <c r="C97" t="s">
+        <v>527</v>
+      </c>
+      <c r="D97" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>384</v>
+      </c>
+      <c r="B98" t="s">
+        <v>479</v>
+      </c>
+      <c r="C98" t="s">
+        <v>528</v>
+      </c>
+      <c r="D98" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>376</v>
+      </c>
+      <c r="B99" t="s">
+        <v>480</v>
+      </c>
+      <c r="C99" t="s">
+        <v>529</v>
+      </c>
+      <c r="D99" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>378</v>
+      </c>
+      <c r="B100" t="s">
+        <v>481</v>
+      </c>
+      <c r="C100" t="s">
+        <v>530</v>
+      </c>
+      <c r="D100" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>378</v>
+      </c>
+      <c r="B101" t="s">
+        <v>482</v>
+      </c>
+      <c r="C101" t="s">
+        <v>531</v>
+      </c>
+      <c r="D101" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>376</v>
+      </c>
+      <c r="B102" t="s">
+        <v>483</v>
+      </c>
+      <c r="C102" t="s">
+        <v>532</v>
+      </c>
+      <c r="D102" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>378</v>
+      </c>
+      <c r="B103" t="s">
+        <v>484</v>
+      </c>
+      <c r="C103" t="s">
+        <v>424</v>
+      </c>
+      <c r="D103" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>378</v>
+      </c>
+      <c r="B104" t="s">
+        <v>485</v>
+      </c>
+      <c r="C104" t="s">
+        <v>497</v>
+      </c>
+      <c r="D104" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>376</v>
+      </c>
+      <c r="B105" t="s">
+        <v>486</v>
+      </c>
+      <c r="C105" t="s">
+        <v>533</v>
+      </c>
+      <c r="D105" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>376</v>
+      </c>
+      <c r="B106" t="s">
+        <v>487</v>
+      </c>
+      <c r="C106" t="s">
+        <v>534</v>
+      </c>
+      <c r="D106" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>378</v>
+      </c>
+      <c r="B107" t="s">
+        <v>488</v>
+      </c>
+      <c r="C107" t="s">
+        <v>424</v>
+      </c>
+      <c r="D107" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>378</v>
+      </c>
+      <c r="B108" t="s">
+        <v>489</v>
+      </c>
+      <c r="C108" t="s">
+        <v>424</v>
+      </c>
+      <c r="D108" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>379</v>
+      </c>
+      <c r="B109" t="s">
+        <v>490</v>
+      </c>
+      <c r="C109" t="s">
+        <v>535</v>
+      </c>
+      <c r="D109" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>377</v>
+      </c>
+      <c r="B110" t="s">
+        <v>491</v>
+      </c>
+      <c r="C110" t="s">
+        <v>536</v>
+      </c>
+      <c r="D110" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>377</v>
+      </c>
+      <c r="B111" t="s">
+        <v>492</v>
+      </c>
+      <c r="C111" t="s">
+        <v>537</v>
+      </c>
+      <c r="D111" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>383</v>
+      </c>
+      <c r="B112" t="s">
+        <v>493</v>
+      </c>
+      <c r="C112" t="s">
+        <v>538</v>
+      </c>
+      <c r="D112" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>380</v>
+      </c>
+      <c r="B113" t="s">
+        <v>494</v>
+      </c>
+      <c r="C113" t="s">
+        <v>539</v>
+      </c>
+      <c r="D113" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>383</v>
+      </c>
+      <c r="B114" t="s">
+        <v>495</v>
+      </c>
+      <c r="C114" t="s">
+        <v>540</v>
+      </c>
+      <c r="D114" t="s">
+        <v>593</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>